<commit_message>
finish documentation for transfer API identity resolution
</commit_message>
<xml_diff>
--- a/IdentityResolutionExperimentation/identity_resolution_results.xlsx
+++ b/IdentityResolutionExperimentation/identity_resolution_results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26621"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="3200" yWindow="0" windowWidth="25600" windowHeight="16600" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Blatt2" sheetId="2" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="144">
   <si>
     <t>Blocker</t>
   </si>
@@ -448,6 +448,9 @@
   </si>
   <si>
     <t>2 Minutes 25 Seconds</t>
+  </si>
+  <si>
+    <t>0.79</t>
   </si>
 </sst>
 </file>
@@ -504,8 +507,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="71">
+  <cellStyleXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -582,7 +589,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="71">
+  <cellStyles count="75">
     <cellStyle name="Besuchter Link" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="6" builtinId="9" hidden="1"/>
@@ -618,6 +625,8 @@
     <cellStyle name="Besuchter Link" xfId="66" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="68" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="74" builtinId="9" hidden="1"/>
     <cellStyle name="Link" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="5" builtinId="8" hidden="1"/>
@@ -653,6 +662,8 @@
     <cellStyle name="Link" xfId="65" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="67" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="73" builtinId="8" hidden="1"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -982,10 +993,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q60"/>
+  <dimension ref="A1:Q61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D30" workbookViewId="0">
-      <selection activeCell="M59" sqref="M59"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="M61" sqref="M61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1999,7 +2010,7 @@
         <v>9856</v>
       </c>
     </row>
-    <row r="54" spans="1:12">
+    <row r="54" spans="1:13">
       <c r="A54" s="1" t="s">
         <v>32</v>
       </c>
@@ -2014,7 +2025,7 @@
       <c r="J54" s="1"/>
       <c r="K54" s="1"/>
     </row>
-    <row r="55" spans="1:12">
+    <row r="55" spans="1:13">
       <c r="A55" s="1" t="s">
         <v>0</v>
       </c>
@@ -2051,8 +2062,11 @@
       <c r="L55" s="1" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="56" spans="1:12">
+      <c r="M55" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13">
       <c r="A56" t="s">
         <v>18</v>
       </c>
@@ -2089,8 +2103,11 @@
       <c r="L56">
         <v>8841</v>
       </c>
-    </row>
-    <row r="57" spans="1:12">
+      <c r="M56" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13">
       <c r="A57" t="s">
         <v>18</v>
       </c>
@@ -2127,8 +2144,11 @@
       <c r="L57" s="2">
         <v>5590</v>
       </c>
-    </row>
-    <row r="58" spans="1:12">
+      <c r="M57" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13">
       <c r="A58" t="s">
         <v>18</v>
       </c>
@@ -2165,8 +2185,11 @@
       <c r="L58" s="2">
         <v>6912</v>
       </c>
-    </row>
-    <row r="59" spans="1:12">
+      <c r="M58" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13">
       <c r="A59" t="s">
         <v>18</v>
       </c>
@@ -2203,8 +2226,14 @@
       <c r="L59" s="2">
         <v>3286</v>
       </c>
-    </row>
-    <row r="60" spans="1:12">
+      <c r="M59" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13">
+      <c r="A60" t="s">
+        <v>18</v>
+      </c>
       <c r="B60" t="s">
         <v>133</v>
       </c>
@@ -2238,6 +2267,12 @@
       <c r="L60" s="2">
         <v>3367</v>
       </c>
+      <c r="M60" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="61" spans="1:13">
+      <c r="L61" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
work with FIFA _ ESD correspondences
</commit_message>
<xml_diff>
--- a/IdentityResolutionExperimentation/identity_resolution_results.xlsx
+++ b/IdentityResolutionExperimentation/identity_resolution_results.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26621"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22130"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\linar\OneDrive\Документы\GitHub\WDI_2019\IdentityResolutionExperimentation\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9A67258-88FB-432A-A22B-919F375E2AC1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3200" yWindow="0" windowWidth="25600" windowHeight="16600" tabRatio="500"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blatt2" sheetId="2" r:id="rId1"/>
@@ -19,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="152">
   <si>
     <t>Blocker</t>
   </si>
@@ -415,12 +421,72 @@
   </si>
   <si>
     <t>13 Minutes 2 Seconds</t>
+  </si>
+  <si>
+    <t>0.81</t>
+  </si>
+  <si>
+    <t xml:space="preserve">many false correspondences, since the first letter of the  name is the same, the DoB, height and weight are also pretty similar </t>
+  </si>
+  <si>
+    <t>deleting the MaxTokenize - worse, since the similarity for the false correspondences increased</t>
+  </si>
+  <si>
+    <t>0.67</t>
+  </si>
+  <si>
+    <t>decreasing the threshold gave more true correspondences</t>
+  </si>
+  <si>
+    <t>there is some false correspondences, maybe increase the treshold</t>
+  </si>
+  <si>
+    <t>0.9253</t>
+  </si>
+  <si>
+    <t>0.8342</t>
+  </si>
+  <si>
+    <t>0.8774</t>
+  </si>
+  <si>
+    <t>1 Minute 18 Seconds</t>
+  </si>
+  <si>
+    <t>there is some false correspondences, so increase the threshold</t>
+  </si>
+  <si>
+    <t>0.76</t>
+  </si>
+  <si>
+    <t>0.9693</t>
+  </si>
+  <si>
+    <t>0.8187</t>
+  </si>
+  <si>
+    <t>0.8876</t>
+  </si>
+  <si>
+    <t>2 Minutes 33 Seconds</t>
+  </si>
+  <si>
+    <t>0.78</t>
+  </si>
+  <si>
+    <t>0.9688</t>
+  </si>
+  <si>
+    <t>0.8031</t>
+  </si>
+  <si>
+    <t>0.8782</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -454,12 +520,24 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -542,84 +620,95 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="69">
-    <cellStyle name="Besuchter Link" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="16" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="18" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="20" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="22" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="24" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="26" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="28" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="30" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="32" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="34" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="36" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="38" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="40" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="42" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="44" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="46" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="48" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="50" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="52" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="54" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="56" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="58" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="60" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="62" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="64" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="66" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="68" builtinId="9" hidden="1"/>
-    <cellStyle name="Link" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="7" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="9" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="11" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="13" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="15" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="17" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="19" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="21" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="23" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="25" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="27" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="29" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="31" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="33" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="35" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="37" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="39" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="41" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="43" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="45" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="47" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="49" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="51" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="53" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="55" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="57" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="59" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="61" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="63" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="65" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="67" builtinId="8" hidden="1"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Гиперссылка" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="68" builtinId="9" hidden="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -944,14 +1033,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q59"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:R62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+    <sheetView tabSelected="1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="44.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="43.5" bestFit="1" customWidth="1"/>
@@ -968,12 +1057,12 @@
     <col min="15" max="15" width="14.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:17">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1026,7 +1115,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="3" spans="1:17">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -1069,11 +1158,17 @@
       <c r="N3">
         <v>6</v>
       </c>
+      <c r="O3" t="s">
+        <v>132</v>
+      </c>
+      <c r="P3">
+        <v>18246</v>
+      </c>
       <c r="Q3" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="1:17">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>39</v>
       </c>
@@ -1119,11 +1214,14 @@
       <c r="O4" t="s">
         <v>43</v>
       </c>
+      <c r="P4">
+        <v>437</v>
+      </c>
       <c r="Q4" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:17">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -1169,61 +1267,68 @@
       <c r="O5" t="s">
         <v>44</v>
       </c>
+      <c r="P5">
+        <v>18019</v>
+      </c>
       <c r="Q5" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="6" spans="1:17">
-      <c r="A6" t="s">
+      <c r="R5" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A6" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C6">
-        <v>0</v>
-      </c>
-      <c r="D6" t="s">
+      <c r="C6" s="3">
+        <v>0</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E6">
-        <v>0</v>
-      </c>
-      <c r="F6">
-        <v>0</v>
-      </c>
-      <c r="G6" t="s">
-        <v>31</v>
-      </c>
-      <c r="H6" t="s">
-        <v>31</v>
-      </c>
-      <c r="I6" t="s">
+      <c r="E6" s="3">
+        <v>0</v>
+      </c>
+      <c r="F6" s="3">
+        <v>0</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="I6" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="J6" t="s">
+      <c r="J6" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="K6" t="s">
+      <c r="K6" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="L6" t="s">
+      <c r="L6" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="M6" t="s">
+      <c r="M6" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="N6">
+      <c r="N6" s="3">
         <v>7</v>
       </c>
-      <c r="O6" t="s">
+      <c r="O6" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="Q6" t="s">
+      <c r="P6" s="3"/>
+      <c r="Q6" s="3" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="1:17">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -1269,175 +1374,191 @@
       <c r="O7" t="s">
         <v>44</v>
       </c>
+      <c r="P7">
+        <v>11468</v>
+      </c>
       <c r="Q7" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="8" spans="1:17">
-      <c r="A8" t="s">
+      <c r="R7" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A8" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B8">
-        <v>0</v>
-      </c>
-      <c r="C8">
-        <v>0</v>
-      </c>
-      <c r="D8">
-        <v>0</v>
-      </c>
-      <c r="E8">
-        <v>0</v>
-      </c>
-      <c r="F8" t="s">
+      <c r="B8" s="4">
+        <v>0</v>
+      </c>
+      <c r="C8" s="4">
+        <v>0</v>
+      </c>
+      <c r="D8" s="4">
+        <v>0</v>
+      </c>
+      <c r="E8" s="4">
+        <v>0</v>
+      </c>
+      <c r="F8" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="G8" t="s">
-        <v>31</v>
-      </c>
-      <c r="H8" t="s">
-        <v>31</v>
-      </c>
-      <c r="I8" t="s">
+      <c r="G8" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="I8" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="J8" t="s">
+      <c r="J8" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="K8" t="s">
+      <c r="K8" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="L8" t="s">
+      <c r="L8" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="M8" t="s">
+      <c r="M8" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="N8">
+      <c r="N8" s="4">
         <v>26</v>
       </c>
-      <c r="O8" t="s">
+      <c r="O8" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="Q8" t="s">
+      <c r="P8" s="4">
+        <v>4010</v>
+      </c>
+      <c r="Q8" s="4" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:17">
-      <c r="A9" t="s">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A9" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="4">
+        <v>0</v>
+      </c>
+      <c r="C9" s="4">
+        <v>0</v>
+      </c>
+      <c r="D9" s="4">
+        <v>0</v>
+      </c>
+      <c r="E9" s="4">
+        <v>0</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="I9" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="J9" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="K9" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="L9" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="M9" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="N9" s="4">
+        <v>26</v>
+      </c>
+      <c r="O9" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="P9" s="4">
+        <v>4238</v>
+      </c>
+      <c r="Q9" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="R9" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A10" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C9">
-        <v>0</v>
-      </c>
-      <c r="D9" t="s">
+      <c r="C10" s="3">
+        <v>0</v>
+      </c>
+      <c r="D10" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E9">
-        <v>0</v>
-      </c>
-      <c r="F9">
-        <v>0</v>
-      </c>
-      <c r="G9" t="s">
+      <c r="E10" s="3">
+        <v>0</v>
+      </c>
+      <c r="F10" s="3">
+        <v>0</v>
+      </c>
+      <c r="G10" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="H9" t="s">
+      <c r="H10" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="I9" t="s">
+      <c r="I10" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="J9" t="s">
+      <c r="J10" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="K9" t="s">
+      <c r="K10" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="L9" t="s">
+      <c r="L10" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="M9" t="s">
+      <c r="M10" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="N9">
+      <c r="N10" s="3">
         <v>26</v>
       </c>
-      <c r="O9" t="s">
+      <c r="O10" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="Q9" t="s">
+      <c r="P10" s="3"/>
+      <c r="Q10" s="3" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="10" spans="1:17">
-      <c r="A10" t="s">
-        <v>18</v>
-      </c>
-      <c r="B10">
-        <v>0</v>
-      </c>
-      <c r="C10">
-        <v>0</v>
-      </c>
-      <c r="D10">
-        <v>0</v>
-      </c>
-      <c r="E10" t="s">
-        <v>62</v>
-      </c>
-      <c r="F10">
-        <v>0</v>
-      </c>
-      <c r="G10" t="s">
-        <v>31</v>
-      </c>
-      <c r="H10" t="s">
-        <v>31</v>
-      </c>
-      <c r="I10" t="s">
-        <v>4</v>
-      </c>
-      <c r="J10" t="s">
-        <v>72</v>
-      </c>
-      <c r="K10" t="s">
-        <v>83</v>
-      </c>
-      <c r="L10" t="s">
-        <v>73</v>
-      </c>
-      <c r="M10" t="s">
-        <v>74</v>
-      </c>
-      <c r="N10">
-        <v>26</v>
-      </c>
-      <c r="O10" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q10" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>18</v>
       </c>
-      <c r="B11" t="s">
-        <v>31</v>
+      <c r="B11">
+        <v>0</v>
       </c>
       <c r="C11">
         <v>0</v>
       </c>
-      <c r="D11" t="s">
-        <v>31</v>
-      </c>
-      <c r="E11">
-        <v>0</v>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11" t="s">
+        <v>62</v>
       </c>
       <c r="F11">
         <v>0</v>
@@ -1452,16 +1573,16 @@
         <v>4</v>
       </c>
       <c r="J11" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="K11" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="L11" t="s">
-        <v>88</v>
+        <v>73</v>
       </c>
       <c r="M11" t="s">
-        <v>92</v>
+        <v>74</v>
       </c>
       <c r="N11">
         <v>26</v>
@@ -1469,677 +1590,849 @@
       <c r="O11" t="s">
         <v>44</v>
       </c>
+      <c r="P11">
+        <v>4199</v>
+      </c>
       <c r="Q11" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="12" spans="1:17">
-      <c r="A12" t="s">
+      <c r="R11" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A12" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12" s="4">
+        <v>0</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="E12" s="4">
+        <v>0</v>
+      </c>
+      <c r="F12" s="4">
+        <v>0</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="I12" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="J12" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="K12" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="L12" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="M12" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="N12" s="4">
+        <v>26</v>
+      </c>
+      <c r="O12" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="P12" s="4">
+        <v>21468</v>
+      </c>
+      <c r="Q12" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="R12" s="4" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A13" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C13" s="4">
+        <v>0</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="E13" s="4">
+        <v>0</v>
+      </c>
+      <c r="F13" s="4">
+        <v>0</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="I13" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="J13" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="K13" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="L13" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="M13" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="N13" s="4">
+        <v>26</v>
+      </c>
+      <c r="O13" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="P13" s="4">
+        <v>4546</v>
+      </c>
+      <c r="Q13" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="R13" s="4"/>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A14" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14" s="4">
+        <v>0</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="E14" s="4">
+        <v>0</v>
+      </c>
+      <c r="F14" s="4">
+        <v>0</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="H14" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="I14" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="J14" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="K14" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="L14" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="M14" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="N14" s="4">
+        <v>26</v>
+      </c>
+      <c r="O14" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="P14" s="4">
+        <v>3944</v>
+      </c>
+      <c r="Q14" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="R14" s="4"/>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
         <v>79</v>
       </c>
-      <c r="B12">
-        <v>0</v>
-      </c>
-      <c r="E12" t="s">
+      <c r="B15">
+        <v>0</v>
+      </c>
+      <c r="E15" t="s">
         <v>62</v>
       </c>
-      <c r="F12">
-        <v>0</v>
-      </c>
-      <c r="G12" t="s">
-        <v>31</v>
-      </c>
-      <c r="H12" t="s">
-        <v>31</v>
-      </c>
-      <c r="I12" t="s">
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15" t="s">
+        <v>31</v>
+      </c>
+      <c r="H15" t="s">
+        <v>31</v>
+      </c>
+      <c r="I15" t="s">
         <v>4</v>
       </c>
-      <c r="J12" t="s">
+      <c r="J15" t="s">
         <v>84</v>
       </c>
-      <c r="K12" t="s">
+      <c r="K15" t="s">
         <v>85</v>
       </c>
-      <c r="L12" t="s">
+      <c r="L15" t="s">
         <v>86</v>
       </c>
-      <c r="M12" t="s">
+      <c r="M15" t="s">
         <v>77</v>
       </c>
-      <c r="N12">
+      <c r="N15">
         <v>18</v>
       </c>
-      <c r="O12" t="s">
+      <c r="O15" t="s">
         <v>80</v>
-      </c>
-      <c r="Q12" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17">
-      <c r="A13" t="s">
-        <v>79</v>
-      </c>
-      <c r="B13" t="s">
-        <v>21</v>
-      </c>
-      <c r="C13">
-        <v>0</v>
-      </c>
-      <c r="D13" t="s">
-        <v>20</v>
-      </c>
-      <c r="E13">
-        <v>0</v>
-      </c>
-      <c r="F13">
-        <v>0</v>
-      </c>
-      <c r="G13" t="s">
-        <v>31</v>
-      </c>
-      <c r="H13" t="s">
-        <v>31</v>
-      </c>
-      <c r="I13" t="s">
-        <v>4</v>
-      </c>
-      <c r="J13" t="s">
-        <v>93</v>
-      </c>
-      <c r="K13" t="s">
-        <v>94</v>
-      </c>
-      <c r="L13" t="s">
-        <v>95</v>
-      </c>
-      <c r="M13" t="s">
-        <v>96</v>
-      </c>
-      <c r="N13">
-        <v>18</v>
-      </c>
-      <c r="O13" t="s">
-        <v>80</v>
-      </c>
-      <c r="Q13" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17">
-      <c r="A14" t="s">
-        <v>18</v>
-      </c>
-      <c r="B14" t="s">
-        <v>31</v>
-      </c>
-      <c r="D14" t="s">
-        <v>31</v>
-      </c>
-      <c r="E14">
-        <v>0</v>
-      </c>
-      <c r="F14">
-        <v>0</v>
-      </c>
-      <c r="G14" t="s">
-        <v>31</v>
-      </c>
-      <c r="H14" t="s">
-        <v>28</v>
-      </c>
-      <c r="I14" t="s">
-        <v>4</v>
-      </c>
-      <c r="J14" t="s">
-        <v>97</v>
-      </c>
-      <c r="K14" t="s">
-        <v>98</v>
-      </c>
-      <c r="L14" t="s">
-        <v>99</v>
-      </c>
-      <c r="M14" t="s">
-        <v>100</v>
-      </c>
-      <c r="N14">
-        <v>26</v>
-      </c>
-      <c r="O14" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q14" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17">
-      <c r="A15" t="s">
-        <v>18</v>
-      </c>
-      <c r="I15" t="s">
-        <v>106</v>
-      </c>
-      <c r="J15">
-        <v>1</v>
-      </c>
-      <c r="K15" t="s">
-        <v>108</v>
-      </c>
-      <c r="L15" t="s">
-        <v>109</v>
-      </c>
-      <c r="M15" t="s">
-        <v>110</v>
-      </c>
-      <c r="N15">
-        <v>26</v>
-      </c>
-      <c r="O15" t="s">
-        <v>44</v>
       </c>
       <c r="Q15" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="16" spans="1:17">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
+        <v>79</v>
+      </c>
+      <c r="B16" t="s">
+        <v>21</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16" t="s">
+        <v>20</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="G16" t="s">
+        <v>31</v>
+      </c>
+      <c r="H16" t="s">
+        <v>31</v>
+      </c>
+      <c r="I16" t="s">
+        <v>4</v>
+      </c>
+      <c r="J16" t="s">
+        <v>93</v>
+      </c>
+      <c r="K16" t="s">
+        <v>94</v>
+      </c>
+      <c r="L16" t="s">
+        <v>95</v>
+      </c>
+      <c r="M16" t="s">
+        <v>96</v>
+      </c>
+      <c r="N16">
         <v>18</v>
       </c>
-      <c r="I16" t="s">
-        <v>118</v>
-      </c>
-      <c r="J16" t="s">
-        <v>119</v>
-      </c>
-      <c r="K16" t="s">
-        <v>120</v>
-      </c>
-      <c r="L16" t="s">
-        <v>121</v>
-      </c>
-      <c r="M16" t="s">
-        <v>122</v>
-      </c>
-      <c r="N16">
-        <v>26</v>
-      </c>
       <c r="O16" t="s">
-        <v>44</v>
-      </c>
-      <c r="P16">
-        <v>14002</v>
+        <v>80</v>
       </c>
       <c r="Q16" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="38" spans="1:14">
-      <c r="A38" s="1" t="s">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A17" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E17" s="5">
+        <v>0</v>
+      </c>
+      <c r="F17" s="5">
+        <v>0</v>
+      </c>
+      <c r="G17" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="H17" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="I17" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="J17" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="K17" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="L17" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="M17" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="N17" s="5">
+        <v>26</v>
+      </c>
+      <c r="O17" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="P17" s="5"/>
+      <c r="Q17" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>18</v>
+      </c>
+      <c r="I18" t="s">
+        <v>106</v>
+      </c>
+      <c r="J18">
+        <v>1</v>
+      </c>
+      <c r="K18" t="s">
+        <v>108</v>
+      </c>
+      <c r="L18" t="s">
+        <v>109</v>
+      </c>
+      <c r="M18" t="s">
+        <v>110</v>
+      </c>
+      <c r="N18">
+        <v>26</v>
+      </c>
+      <c r="O18" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>18</v>
+      </c>
+      <c r="I19" t="s">
+        <v>118</v>
+      </c>
+      <c r="J19" t="s">
+        <v>119</v>
+      </c>
+      <c r="K19" t="s">
+        <v>120</v>
+      </c>
+      <c r="L19" t="s">
+        <v>121</v>
+      </c>
+      <c r="M19" t="s">
+        <v>122</v>
+      </c>
+      <c r="N19">
+        <v>26</v>
+      </c>
+      <c r="O19" t="s">
+        <v>44</v>
+      </c>
+      <c r="P19">
+        <v>14002</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A41" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B38" s="1"/>
-      <c r="C38" s="1"/>
-      <c r="D38" s="1"/>
-      <c r="E38" s="1"/>
-      <c r="F38" s="1"/>
-      <c r="G38" s="1"/>
-      <c r="H38" s="1"/>
-      <c r="I38" s="1"/>
-      <c r="J38" s="1"/>
-      <c r="K38" s="1"/>
-      <c r="L38" s="1"/>
-      <c r="M38" s="1"/>
-    </row>
-    <row r="39" spans="1:14">
-      <c r="A39" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B39" s="1" t="s">
+      <c r="B41" s="1"/>
+      <c r="C41" s="1"/>
+      <c r="D41" s="1"/>
+      <c r="E41" s="1"/>
+      <c r="F41" s="1"/>
+      <c r="G41" s="1"/>
+      <c r="H41" s="1"/>
+      <c r="I41" s="1"/>
+      <c r="J41" s="1"/>
+      <c r="K41" s="1"/>
+      <c r="L41" s="1"/>
+      <c r="M41" s="1"/>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A42" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B42" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C39" s="1" t="s">
+      <c r="C42" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D39" s="1" t="s">
+      <c r="D42" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E39" s="1" t="s">
+      <c r="E42" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F39" s="1" t="s">
+      <c r="F42" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="G39" s="1" t="s">
+      <c r="G42" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="H39" s="1" t="s">
+      <c r="H42" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="I39" s="1" t="s">
+      <c r="I42" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="J39" s="1" t="s">
+      <c r="J42" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="K39" s="1" t="s">
+      <c r="K42" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="L39" s="1" t="s">
+      <c r="L42" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="M39" s="1" t="s">
+      <c r="M42" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="N39" s="1" t="s">
+      <c r="N42" s="1" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="40" spans="1:14">
-      <c r="A40" t="s">
+    <row r="43" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
         <v>18</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B43" t="s">
         <v>19</v>
       </c>
-      <c r="C40">
-        <v>0</v>
-      </c>
-      <c r="D40" t="s">
+      <c r="C43">
+        <v>0</v>
+      </c>
+      <c r="D43" t="s">
         <v>21</v>
       </c>
-      <c r="E40" t="s">
+      <c r="E43" t="s">
         <v>20</v>
       </c>
-      <c r="F40">
-        <v>0</v>
-      </c>
-      <c r="G40" t="s">
-        <v>4</v>
-      </c>
-      <c r="H40" t="s">
-        <v>22</v>
-      </c>
-      <c r="I40" t="s">
-        <v>23</v>
-      </c>
-      <c r="J40" t="s">
-        <v>24</v>
-      </c>
-      <c r="K40" t="s">
-        <v>25</v>
-      </c>
-      <c r="L40">
-        <v>26</v>
-      </c>
-      <c r="M40" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="41" spans="1:14">
-      <c r="A41" t="s">
-        <v>18</v>
-      </c>
-      <c r="B41">
-        <v>0</v>
-      </c>
-      <c r="C41" t="s">
-        <v>19</v>
-      </c>
-      <c r="D41" t="s">
-        <v>21</v>
-      </c>
-      <c r="E41">
-        <v>0</v>
-      </c>
-      <c r="F41" t="s">
-        <v>20</v>
-      </c>
-      <c r="G41" t="s">
-        <v>4</v>
-      </c>
-      <c r="H41" t="s">
-        <v>47</v>
-      </c>
-      <c r="I41" t="s">
-        <v>48</v>
-      </c>
-      <c r="J41" t="s">
-        <v>49</v>
-      </c>
-      <c r="K41" t="s">
-        <v>50</v>
-      </c>
-      <c r="L41">
-        <v>26</v>
-      </c>
-      <c r="M41" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="42" spans="1:14">
-      <c r="A42" t="s">
-        <v>78</v>
-      </c>
-      <c r="K42" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="43" spans="1:14">
-      <c r="A43" t="s">
-        <v>79</v>
-      </c>
-      <c r="B43" t="s">
-        <v>21</v>
-      </c>
-      <c r="D43" t="s">
-        <v>20</v>
-      </c>
-      <c r="F43" t="s">
-        <v>62</v>
+      <c r="F43">
+        <v>0</v>
       </c>
       <c r="G43" t="s">
         <v>4</v>
       </c>
       <c r="H43" t="s">
-        <v>66</v>
+        <v>22</v>
       </c>
       <c r="I43" t="s">
-        <v>89</v>
+        <v>23</v>
       </c>
       <c r="J43" t="s">
-        <v>90</v>
+        <v>24</v>
       </c>
       <c r="K43" t="s">
-        <v>91</v>
+        <v>25</v>
       </c>
       <c r="L43">
+        <v>26</v>
+      </c>
+      <c r="M43" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
+        <v>18</v>
+      </c>
+      <c r="B44">
+        <v>0</v>
+      </c>
+      <c r="C44" t="s">
+        <v>19</v>
+      </c>
+      <c r="D44" t="s">
+        <v>21</v>
+      </c>
+      <c r="E44">
+        <v>0</v>
+      </c>
+      <c r="F44" t="s">
         <v>20</v>
-      </c>
-      <c r="M43" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="44" spans="1:14">
-      <c r="A44" t="s">
-        <v>79</v>
-      </c>
-      <c r="C44" t="s">
-        <v>21</v>
-      </c>
-      <c r="D44" t="s">
-        <v>20</v>
-      </c>
-      <c r="E44" t="s">
-        <v>62</v>
       </c>
       <c r="G44" t="s">
         <v>4</v>
       </c>
       <c r="H44" t="s">
+        <v>47</v>
+      </c>
+      <c r="I44" t="s">
+        <v>48</v>
+      </c>
+      <c r="J44" t="s">
+        <v>49</v>
+      </c>
+      <c r="K44" t="s">
+        <v>50</v>
+      </c>
+      <c r="L44">
+        <v>26</v>
+      </c>
+      <c r="M44" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
+        <v>78</v>
+      </c>
+      <c r="K45" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A46" t="s">
+        <v>79</v>
+      </c>
+      <c r="B46" t="s">
+        <v>21</v>
+      </c>
+      <c r="D46" t="s">
+        <v>20</v>
+      </c>
+      <c r="F46" t="s">
+        <v>62</v>
+      </c>
+      <c r="G46" t="s">
+        <v>4</v>
+      </c>
+      <c r="H46" t="s">
+        <v>66</v>
+      </c>
+      <c r="I46" t="s">
+        <v>89</v>
+      </c>
+      <c r="J46" t="s">
+        <v>90</v>
+      </c>
+      <c r="K46" t="s">
+        <v>91</v>
+      </c>
+      <c r="L46">
+        <v>20</v>
+      </c>
+      <c r="M46" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
+        <v>79</v>
+      </c>
+      <c r="C47" t="s">
+        <v>21</v>
+      </c>
+      <c r="D47" t="s">
+        <v>20</v>
+      </c>
+      <c r="E47" t="s">
+        <v>62</v>
+      </c>
+      <c r="G47" t="s">
+        <v>4</v>
+      </c>
+      <c r="H47" t="s">
         <v>102</v>
       </c>
-      <c r="I44" t="s">
+      <c r="I47" t="s">
         <v>89</v>
       </c>
-      <c r="J44" t="s">
+      <c r="J47" t="s">
         <v>103</v>
       </c>
-      <c r="K44" t="s">
+      <c r="K47" t="s">
         <v>104</v>
       </c>
-      <c r="L44">
+      <c r="L47">
         <v>20</v>
       </c>
-      <c r="M44" t="s">
+      <c r="M47" t="s">
         <v>105</v>
       </c>
-      <c r="N44">
+      <c r="N47">
         <v>1162680</v>
       </c>
     </row>
-    <row r="45" spans="1:14">
-      <c r="A45" t="s">
+    <row r="48" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A48" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="46" spans="1:14">
-      <c r="A46" t="s">
+    <row r="49" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A49" t="s">
         <v>18</v>
       </c>
-      <c r="G46" t="s">
+      <c r="G49" t="s">
         <v>123</v>
       </c>
-      <c r="H46">
+      <c r="H49">
         <v>1</v>
       </c>
-      <c r="I46" t="s">
+      <c r="I49" t="s">
         <v>124</v>
       </c>
-      <c r="J46" t="s">
+      <c r="J49" t="s">
         <v>125</v>
       </c>
-      <c r="K46" t="s">
+      <c r="K49" t="s">
         <v>126</v>
       </c>
-      <c r="L46">
+      <c r="L49">
         <v>26</v>
       </c>
-      <c r="M46" t="s">
+      <c r="M49" t="s">
         <v>44</v>
       </c>
-      <c r="N46">
+      <c r="N49">
         <v>9931</v>
       </c>
     </row>
-    <row r="47" spans="1:14">
-      <c r="A47" t="s">
+    <row r="50" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A50" t="s">
         <v>18</v>
       </c>
-      <c r="G47" t="s">
+      <c r="G50" t="s">
         <v>123</v>
       </c>
-      <c r="H47">
+      <c r="H50">
         <v>1</v>
       </c>
-      <c r="I47" t="s">
+      <c r="I50" t="s">
         <v>124</v>
       </c>
-      <c r="J47" t="s">
+      <c r="J50" t="s">
         <v>125</v>
       </c>
-      <c r="K47" t="s">
+      <c r="K50" t="s">
         <v>131</v>
       </c>
-      <c r="L47">
+      <c r="L50">
         <v>26</v>
       </c>
-      <c r="M47" t="s">
+      <c r="M50" t="s">
         <v>44</v>
       </c>
-      <c r="N47">
+      <c r="N50">
         <v>9856</v>
       </c>
     </row>
-    <row r="54" spans="1:12">
-      <c r="A54" s="1" t="s">
+    <row r="57" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A57" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B54" s="1"/>
-      <c r="C54" s="1"/>
-      <c r="D54" s="1"/>
-      <c r="E54" s="1"/>
-      <c r="F54" s="1"/>
-      <c r="G54" s="1"/>
-      <c r="H54" s="1"/>
-      <c r="I54" s="1"/>
-      <c r="J54" s="1"/>
-      <c r="K54" s="1"/>
-    </row>
-    <row r="55" spans="1:12">
-      <c r="A55" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B55" s="1" t="s">
+      <c r="B57" s="1"/>
+      <c r="C57" s="1"/>
+      <c r="D57" s="1"/>
+      <c r="E57" s="1"/>
+      <c r="F57" s="1"/>
+      <c r="G57" s="1"/>
+      <c r="H57" s="1"/>
+      <c r="I57" s="1"/>
+      <c r="J57" s="1"/>
+      <c r="K57" s="1"/>
+    </row>
+    <row r="58" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A58" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B58" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C55" s="1" t="s">
+      <c r="C58" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D55" s="1" t="s">
+      <c r="D58" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E55" s="1" t="s">
+      <c r="E58" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F55" s="1" t="s">
+      <c r="F58" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="G55" s="1" t="s">
+      <c r="G58" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="H55" s="1" t="s">
+      <c r="H58" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="I55" s="1" t="s">
+      <c r="I58" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="J55" s="1" t="s">
+      <c r="J58" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="K55" s="1" t="s">
+      <c r="K58" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="L55" s="1" t="s">
+      <c r="L58" s="1" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="56" spans="1:12">
-      <c r="A56" t="s">
-        <v>18</v>
-      </c>
-      <c r="B56" t="s">
-        <v>34</v>
-      </c>
-      <c r="C56">
-        <v>0</v>
-      </c>
-      <c r="D56" t="s">
-        <v>21</v>
-      </c>
-      <c r="E56" t="s">
-        <v>4</v>
-      </c>
-      <c r="F56" t="s">
-        <v>35</v>
-      </c>
-      <c r="G56" t="s">
-        <v>36</v>
-      </c>
-      <c r="H56" t="s">
-        <v>37</v>
-      </c>
-      <c r="I56" t="s">
-        <v>38</v>
-      </c>
-      <c r="J56">
-        <v>26</v>
-      </c>
-      <c r="K56" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="57" spans="1:12">
-      <c r="A57" t="s">
-        <v>18</v>
-      </c>
-      <c r="B57" t="s">
-        <v>34</v>
-      </c>
-      <c r="C57" t="s">
-        <v>34</v>
-      </c>
-      <c r="D57" t="s">
-        <v>21</v>
-      </c>
-      <c r="E57" t="s">
-        <v>4</v>
-      </c>
-      <c r="F57" t="s">
-        <v>113</v>
-      </c>
-      <c r="G57" t="s">
-        <v>114</v>
-      </c>
-      <c r="H57" t="s">
-        <v>115</v>
-      </c>
-      <c r="I57" t="s">
-        <v>116</v>
-      </c>
-      <c r="J57">
-        <v>26</v>
-      </c>
-      <c r="K57" t="s">
-        <v>117</v>
-      </c>
-      <c r="L57" s="2">
-        <v>5590</v>
-      </c>
-    </row>
-    <row r="58" spans="1:12">
-      <c r="A58" t="s">
-        <v>18</v>
-      </c>
-      <c r="B58" t="s">
-        <v>112</v>
-      </c>
-      <c r="C58">
-        <v>0</v>
-      </c>
-      <c r="D58" t="s">
-        <v>71</v>
-      </c>
-      <c r="E58" t="s">
-        <v>4</v>
-      </c>
-      <c r="F58" t="s">
-        <v>127</v>
-      </c>
-      <c r="G58" t="s">
-        <v>128</v>
-      </c>
-      <c r="H58" t="s">
-        <v>129</v>
-      </c>
-      <c r="I58" t="s">
-        <v>130</v>
-      </c>
-      <c r="J58">
-        <v>26</v>
-      </c>
-      <c r="K58" t="s">
-        <v>117</v>
-      </c>
-      <c r="L58" s="2">
-        <v>6912</v>
-      </c>
-    </row>
-    <row r="59" spans="1:12">
+    <row r="59" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>18</v>
       </c>
-      <c r="B59">
-        <v>0</v>
+      <c r="B59" t="s">
+        <v>34</v>
+      </c>
+      <c r="C59">
+        <v>0</v>
+      </c>
+      <c r="D59" t="s">
+        <v>21</v>
       </c>
       <c r="E59" t="s">
         <v>4</v>
       </c>
+      <c r="F59" t="s">
+        <v>35</v>
+      </c>
+      <c r="G59" t="s">
+        <v>36</v>
+      </c>
+      <c r="H59" t="s">
+        <v>37</v>
+      </c>
+      <c r="I59" t="s">
+        <v>38</v>
+      </c>
       <c r="J59">
         <v>26</v>
       </c>
       <c r="K59" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="60" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A60" t="s">
+        <v>18</v>
+      </c>
+      <c r="B60" t="s">
+        <v>34</v>
+      </c>
+      <c r="C60" t="s">
+        <v>34</v>
+      </c>
+      <c r="D60" t="s">
+        <v>21</v>
+      </c>
+      <c r="E60" t="s">
+        <v>4</v>
+      </c>
+      <c r="F60" t="s">
+        <v>113</v>
+      </c>
+      <c r="G60" t="s">
+        <v>114</v>
+      </c>
+      <c r="H60" t="s">
+        <v>115</v>
+      </c>
+      <c r="I60" t="s">
+        <v>116</v>
+      </c>
+      <c r="J60">
+        <v>26</v>
+      </c>
+      <c r="K60" t="s">
+        <v>117</v>
+      </c>
+      <c r="L60" s="2">
+        <v>5590</v>
+      </c>
+    </row>
+    <row r="61" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A61" t="s">
+        <v>18</v>
+      </c>
+      <c r="B61" t="s">
+        <v>112</v>
+      </c>
+      <c r="C61">
+        <v>0</v>
+      </c>
+      <c r="D61" t="s">
+        <v>71</v>
+      </c>
+      <c r="E61" t="s">
+        <v>4</v>
+      </c>
+      <c r="F61" t="s">
+        <v>127</v>
+      </c>
+      <c r="G61" t="s">
+        <v>128</v>
+      </c>
+      <c r="H61" t="s">
+        <v>129</v>
+      </c>
+      <c r="I61" t="s">
+        <v>130</v>
+      </c>
+      <c r="J61">
+        <v>26</v>
+      </c>
+      <c r="K61" t="s">
+        <v>117</v>
+      </c>
+      <c r="L61" s="2">
+        <v>6912</v>
+      </c>
+    </row>
+    <row r="62" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A62" t="s">
+        <v>18</v>
+      </c>
+      <c r="B62">
+        <v>0</v>
+      </c>
+      <c r="E62" t="s">
+        <v>4</v>
+      </c>
+      <c r="J62">
+        <v>26</v>
+      </c>
+      <c r="K62" t="s">
         <v>117</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update the FIFA_EU experimentation
</commit_message>
<xml_diff>
--- a/IdentityResolutionExperimentation/identity_resolution_results.xlsx
+++ b/IdentityResolutionExperimentation/identity_resolution_results.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10908"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22130"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maida/Documents/GitHub/WDI_2019/IdentityResolutionExperimentation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\linar\OneDrive\Документы\GitHub\WDI_2019\IdentityResolutionExperimentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB4CEEDD-CB56-D444-9B97-EC6AB1C24203}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEBBE62A-3771-49E5-A375-40ED74B53410}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3200" yWindow="460" windowWidth="25600" windowHeight="16420" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1020" yWindow="2450" windowWidth="14400" windowHeight="7360" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blatt2" sheetId="2" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="162">
   <si>
     <t>Blocker</t>
   </si>
@@ -454,13 +454,70 @@
   </si>
   <si>
     <t>2 Minutes 22 Seconds</t>
+  </si>
+  <si>
+    <t>0.81</t>
+  </si>
+  <si>
+    <t xml:space="preserve">many false correspondences, since the first letter of the  name is the same, the DoB, height and weight are also pretty similar </t>
+  </si>
+  <si>
+    <t>deleting the MaxTokenize - worse, since the similarity for the false correspondences increased</t>
+  </si>
+  <si>
+    <t>0.9253</t>
+  </si>
+  <si>
+    <t>0.8342</t>
+  </si>
+  <si>
+    <t>0.8774</t>
+  </si>
+  <si>
+    <t>1 Minute 18 Seconds</t>
+  </si>
+  <si>
+    <t>0.67</t>
+  </si>
+  <si>
+    <t>decreasing the threshold gave more true correspondences</t>
+  </si>
+  <si>
+    <t>there is some false correspondences, maybe increase the treshold</t>
+  </si>
+  <si>
+    <t>there is some false correspondences, so increase the threshold</t>
+  </si>
+  <si>
+    <t>0.9693</t>
+  </si>
+  <si>
+    <t>0.8187</t>
+  </si>
+  <si>
+    <t>0.8876</t>
+  </si>
+  <si>
+    <t>2 Minutes 33 Seconds</t>
+  </si>
+  <si>
+    <t>0.76</t>
+  </si>
+  <si>
+    <t>0.8031</t>
+  </si>
+  <si>
+    <t>0.8782</t>
+  </si>
+  <si>
+    <t>0.78</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="6">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -603,75 +660,75 @@
     </xf>
   </cellXfs>
   <cellStyles count="69">
-    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Гиперссылка" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="68" builtinId="9" hidden="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -1010,11 +1067,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E33" zoomScale="75" workbookViewId="0">
-      <selection activeCell="O41" sqref="O41"/>
+    <sheetView tabSelected="1" topLeftCell="K7" zoomScale="75" workbookViewId="0">
+      <selection activeCell="U16" sqref="U16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
   <cols>
     <col min="1" max="1" width="44.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="44.33203125" customWidth="1"/>
@@ -1032,270 +1089,288 @@
     <col min="16" max="16" width="14.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:18">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B1" s="1"/>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:18">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1"/>
+      <c r="B2" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="C2" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>37</v>
+        <v>89</v>
       </c>
       <c r="Q2" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="R2" s="1" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="R2" s="1"/>
+    </row>
+    <row r="3" spans="1:18">
       <c r="A3" t="s">
         <v>5</v>
       </c>
-      <c r="C3" t="s">
+      <c r="B3" t="s">
         <v>20</v>
       </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3" t="s">
         <v>19</v>
       </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
       <c r="F3">
         <v>0</v>
       </c>
-      <c r="G3">
-        <v>0</v>
+      <c r="G3" t="s">
+        <v>26</v>
       </c>
       <c r="H3" t="s">
         <v>26</v>
       </c>
       <c r="I3" t="s">
-        <v>26</v>
+        <v>4</v>
       </c>
       <c r="J3" t="s">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="K3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="L3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="M3" t="s">
-        <v>23</v>
-      </c>
-      <c r="N3" t="s">
         <v>24</v>
       </c>
-      <c r="O3">
+      <c r="N3">
         <v>6</v>
       </c>
-      <c r="R3" t="s">
+      <c r="O3" t="s">
+        <v>143</v>
+      </c>
+      <c r="P3">
+        <v>18246</v>
+      </c>
+      <c r="Q3" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:18">
       <c r="A4" t="s">
         <v>34</v>
       </c>
-      <c r="C4" t="s">
+      <c r="B4" t="s">
         <v>20</v>
       </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-      <c r="E4" t="s">
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4" t="s">
         <v>19</v>
       </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
       <c r="F4">
         <v>0</v>
       </c>
-      <c r="G4">
-        <v>0</v>
+      <c r="G4" t="s">
+        <v>26</v>
       </c>
       <c r="H4" t="s">
         <v>26</v>
       </c>
       <c r="I4" t="s">
-        <v>26</v>
-      </c>
-      <c r="J4" t="s">
         <v>4</v>
       </c>
-      <c r="K4">
+      <c r="J4">
         <v>1</v>
       </c>
+      <c r="K4" t="s">
+        <v>35</v>
+      </c>
       <c r="L4" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="M4" t="s">
-        <v>36</v>
-      </c>
-      <c r="N4" t="s">
         <v>40</v>
       </c>
-      <c r="O4">
+      <c r="N4">
         <v>7</v>
       </c>
-      <c r="P4" t="s">
+      <c r="O4" t="s">
         <v>38</v>
       </c>
-      <c r="R4" t="s">
+      <c r="P4">
+        <v>437</v>
+      </c>
+      <c r="Q4" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:18">
       <c r="A5" t="s">
         <v>18</v>
       </c>
-      <c r="C5" t="s">
+      <c r="B5" t="s">
         <v>20</v>
       </c>
-      <c r="D5">
-        <v>0</v>
-      </c>
-      <c r="E5" t="s">
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5" t="s">
         <v>19</v>
       </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
       <c r="F5">
         <v>0</v>
       </c>
-      <c r="G5">
-        <v>0</v>
+      <c r="G5" t="s">
+        <v>26</v>
       </c>
       <c r="H5" t="s">
         <v>26</v>
       </c>
       <c r="I5" t="s">
-        <v>26</v>
+        <v>4</v>
       </c>
       <c r="J5" t="s">
-        <v>4</v>
+        <v>43</v>
       </c>
       <c r="K5" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="L5" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="M5" t="s">
-        <v>45</v>
-      </c>
-      <c r="N5" t="s">
         <v>42</v>
       </c>
-      <c r="O5">
-        <v>26</v>
-      </c>
-      <c r="P5" t="s">
+      <c r="N5">
+        <v>26</v>
+      </c>
+      <c r="O5" t="s">
         <v>39</v>
       </c>
+      <c r="P5">
+        <v>18019</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>29</v>
+      </c>
       <c r="R5" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18">
       <c r="A6" t="s">
         <v>46</v>
       </c>
-      <c r="C6" t="s">
+      <c r="B6" t="s">
         <v>20</v>
       </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-      <c r="E6" t="s">
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6" t="s">
         <v>19</v>
       </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
       <c r="F6">
         <v>0</v>
       </c>
-      <c r="G6">
-        <v>0</v>
+      <c r="G6" t="s">
+        <v>26</v>
       </c>
       <c r="H6" t="s">
         <v>26</v>
       </c>
       <c r="I6" t="s">
-        <v>26</v>
+        <v>4</v>
       </c>
       <c r="J6" t="s">
-        <v>4</v>
+        <v>47</v>
       </c>
       <c r="K6" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="L6" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="M6" t="s">
-        <v>49</v>
-      </c>
-      <c r="N6" t="s">
         <v>50</v>
       </c>
-      <c r="O6">
+      <c r="N6">
         <v>7</v>
       </c>
-      <c r="P6" t="s">
+      <c r="O6" t="s">
         <v>51</v>
       </c>
-      <c r="R6" t="s">
+      <c r="Q6" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:18">
       <c r="A7" t="s">
         <v>18</v>
       </c>
-      <c r="C7" t="s">
+      <c r="B7" t="s">
         <v>53</v>
       </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
       <c r="D7">
         <v>0</v>
       </c>
@@ -1305,44 +1380,50 @@
       <c r="F7">
         <v>0</v>
       </c>
-      <c r="G7">
-        <v>0</v>
+      <c r="G7" t="s">
+        <v>26</v>
       </c>
       <c r="H7" t="s">
         <v>26</v>
       </c>
       <c r="I7" t="s">
-        <v>26</v>
+        <v>4</v>
       </c>
       <c r="J7" t="s">
-        <v>4</v>
+        <v>54</v>
       </c>
       <c r="K7" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="L7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="M7" t="s">
-        <v>56</v>
-      </c>
-      <c r="N7" t="s">
         <v>52</v>
       </c>
-      <c r="O7">
-        <v>26</v>
-      </c>
-      <c r="P7" t="s">
+      <c r="N7">
+        <v>26</v>
+      </c>
+      <c r="O7" t="s">
         <v>39</v>
       </c>
+      <c r="P7">
+        <v>11468</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>29</v>
+      </c>
       <c r="R7" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18">
       <c r="A8" t="s">
         <v>18</v>
       </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
       <c r="C8">
         <v>0</v>
       </c>
@@ -1352,396 +1433,570 @@
       <c r="E8">
         <v>0</v>
       </c>
-      <c r="F8">
-        <v>0</v>
+      <c r="F8" t="s">
+        <v>53</v>
       </c>
       <c r="G8" t="s">
-        <v>53</v>
+        <v>26</v>
       </c>
       <c r="H8" t="s">
         <v>26</v>
       </c>
       <c r="I8" t="s">
-        <v>26</v>
+        <v>4</v>
       </c>
       <c r="J8" t="s">
-        <v>4</v>
+        <v>57</v>
       </c>
       <c r="K8" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="L8" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="M8" t="s">
-        <v>59</v>
-      </c>
-      <c r="N8" t="s">
         <v>60</v>
       </c>
-      <c r="O8">
-        <v>26</v>
-      </c>
-      <c r="P8" t="s">
+      <c r="N8">
+        <v>26</v>
+      </c>
+      <c r="O8" t="s">
         <v>39</v>
       </c>
-      <c r="R8" t="s">
+      <c r="P8">
+        <v>4010</v>
+      </c>
+      <c r="Q8" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:18">
       <c r="A9" t="s">
         <v>18</v>
       </c>
-      <c r="C9" t="s">
-        <v>19</v>
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
       </c>
       <c r="D9">
         <v>0</v>
       </c>
-      <c r="E9" t="s">
-        <v>19</v>
-      </c>
-      <c r="F9">
-        <v>0</v>
-      </c>
-      <c r="G9">
-        <v>0</v>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9" t="s">
+        <v>53</v>
+      </c>
+      <c r="G9" t="s">
+        <v>26</v>
       </c>
       <c r="H9" t="s">
-        <v>61</v>
+        <v>26</v>
       </c>
       <c r="I9" t="s">
-        <v>53</v>
+        <v>4</v>
       </c>
       <c r="J9" t="s">
-        <v>4</v>
+        <v>146</v>
       </c>
       <c r="K9" t="s">
-        <v>66</v>
+        <v>147</v>
       </c>
       <c r="L9" t="s">
-        <v>55</v>
+        <v>148</v>
       </c>
       <c r="M9" t="s">
-        <v>30</v>
-      </c>
-      <c r="N9" t="s">
-        <v>67</v>
-      </c>
-      <c r="O9">
-        <v>26</v>
-      </c>
-      <c r="P9" t="s">
+        <v>149</v>
+      </c>
+      <c r="N9">
+        <v>26</v>
+      </c>
+      <c r="O9" t="s">
         <v>39</v>
       </c>
+      <c r="P9">
+        <v>4238</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>150</v>
+      </c>
       <c r="R9" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18">
       <c r="A10" t="s">
         <v>18</v>
       </c>
+      <c r="B10" t="s">
+        <v>19</v>
+      </c>
       <c r="C10">
         <v>0</v>
       </c>
-      <c r="D10">
-        <v>0</v>
+      <c r="D10" t="s">
+        <v>19</v>
       </c>
       <c r="E10">
         <v>0</v>
       </c>
-      <c r="F10" t="s">
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10" t="s">
+        <v>61</v>
+      </c>
+      <c r="H10" t="s">
         <v>53</v>
       </c>
-      <c r="G10">
-        <v>0</v>
-      </c>
-      <c r="H10" t="s">
-        <v>26</v>
-      </c>
       <c r="I10" t="s">
-        <v>26</v>
+        <v>4</v>
       </c>
       <c r="J10" t="s">
-        <v>4</v>
+        <v>66</v>
       </c>
       <c r="K10" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="L10" t="s">
-        <v>73</v>
+        <v>30</v>
       </c>
       <c r="M10" t="s">
-        <v>63</v>
-      </c>
-      <c r="N10" t="s">
-        <v>64</v>
-      </c>
-      <c r="O10">
-        <v>26</v>
-      </c>
-      <c r="P10" t="s">
+        <v>67</v>
+      </c>
+      <c r="N10">
+        <v>26</v>
+      </c>
+      <c r="O10" t="s">
         <v>39</v>
       </c>
-      <c r="R10" t="s">
+      <c r="Q10" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:18">
       <c r="A11" t="s">
         <v>18</v>
       </c>
-      <c r="C11" t="s">
-        <v>26</v>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
       </c>
       <c r="D11">
         <v>0</v>
       </c>
       <c r="E11" t="s">
-        <v>26</v>
+        <v>53</v>
       </c>
       <c r="F11">
         <v>0</v>
       </c>
-      <c r="G11">
-        <v>0</v>
+      <c r="G11" t="s">
+        <v>26</v>
       </c>
       <c r="H11" t="s">
         <v>26</v>
       </c>
       <c r="I11" t="s">
-        <v>26</v>
+        <v>4</v>
       </c>
       <c r="J11" t="s">
+        <v>62</v>
+      </c>
+      <c r="K11" t="s">
+        <v>73</v>
+      </c>
+      <c r="L11" t="s">
+        <v>63</v>
+      </c>
+      <c r="M11" t="s">
+        <v>64</v>
+      </c>
+      <c r="N11">
+        <v>26</v>
+      </c>
+      <c r="O11" t="s">
+        <v>39</v>
+      </c>
+      <c r="P11">
+        <v>4199</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>29</v>
+      </c>
+      <c r="R11" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18">
+      <c r="A12" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12" t="s">
+        <v>26</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12" t="s">
+        <v>26</v>
+      </c>
+      <c r="H12" t="s">
+        <v>26</v>
+      </c>
+      <c r="I12" t="s">
         <v>4</v>
       </c>
-      <c r="K11" t="s">
+      <c r="J12" t="s">
         <v>72</v>
       </c>
-      <c r="L11" t="s">
+      <c r="K12" t="s">
         <v>77</v>
       </c>
-      <c r="M11" t="s">
+      <c r="L12" t="s">
         <v>78</v>
       </c>
-      <c r="N11" t="s">
+      <c r="M12" t="s">
         <v>80</v>
       </c>
-      <c r="O11">
-        <v>26</v>
-      </c>
-      <c r="P11" t="s">
+      <c r="N12">
+        <v>26</v>
+      </c>
+      <c r="O12" t="s">
         <v>39</v>
       </c>
-      <c r="R11" t="s">
+      <c r="P12">
+        <v>21468</v>
+      </c>
+      <c r="Q12" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>69</v>
-      </c>
-      <c r="C12">
-        <v>0</v>
-      </c>
-      <c r="F12" t="s">
-        <v>53</v>
-      </c>
-      <c r="G12">
-        <v>0</v>
-      </c>
-      <c r="H12" t="s">
-        <v>26</v>
-      </c>
-      <c r="I12" t="s">
-        <v>26</v>
-      </c>
-      <c r="J12" t="s">
+      <c r="R12" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18">
+      <c r="A13" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13" t="s">
+        <v>26</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13" t="s">
+        <v>26</v>
+      </c>
+      <c r="H13" t="s">
+        <v>26</v>
+      </c>
+      <c r="I13" t="s">
         <v>4</v>
       </c>
-      <c r="K12" t="s">
-        <v>74</v>
-      </c>
-      <c r="L12" t="s">
-        <v>75</v>
-      </c>
-      <c r="M12" t="s">
-        <v>76</v>
-      </c>
-      <c r="N12" t="s">
-        <v>67</v>
-      </c>
-      <c r="O12">
-        <v>18</v>
-      </c>
-      <c r="P12" t="s">
-        <v>70</v>
-      </c>
-      <c r="R12" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>69</v>
-      </c>
-      <c r="C13" t="s">
-        <v>20</v>
-      </c>
-      <c r="D13">
-        <v>0</v>
-      </c>
-      <c r="E13" t="s">
-        <v>19</v>
-      </c>
-      <c r="F13">
-        <v>0</v>
-      </c>
-      <c r="G13">
-        <v>0</v>
-      </c>
-      <c r="H13" t="s">
-        <v>26</v>
-      </c>
-      <c r="I13" t="s">
-        <v>26</v>
-      </c>
       <c r="J13" t="s">
-        <v>4</v>
+        <v>154</v>
       </c>
       <c r="K13" t="s">
-        <v>81</v>
+        <v>155</v>
       </c>
       <c r="L13" t="s">
-        <v>82</v>
+        <v>156</v>
       </c>
       <c r="M13" t="s">
-        <v>83</v>
-      </c>
-      <c r="N13" t="s">
-        <v>84</v>
-      </c>
-      <c r="O13">
-        <v>18</v>
-      </c>
-      <c r="P13" t="s">
-        <v>70</v>
-      </c>
-      <c r="R13" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
+        <v>157</v>
+      </c>
+      <c r="N13">
+        <v>26</v>
+      </c>
+      <c r="O13" t="s">
+        <v>39</v>
+      </c>
+      <c r="P13">
+        <v>4546</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18">
       <c r="A14" t="s">
         <v>18</v>
       </c>
-      <c r="C14" t="s">
-        <v>26</v>
-      </c>
-      <c r="E14" t="s">
-        <v>26</v>
+      <c r="B14" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14" t="s">
+        <v>26</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
       </c>
       <c r="F14">
         <v>0</v>
       </c>
-      <c r="G14">
-        <v>0</v>
+      <c r="G14" t="s">
+        <v>26</v>
       </c>
       <c r="H14" t="s">
         <v>26</v>
       </c>
       <c r="I14" t="s">
+        <v>4</v>
+      </c>
+      <c r="J14" t="s">
+        <v>131</v>
+      </c>
+      <c r="K14" t="s">
+        <v>159</v>
+      </c>
+      <c r="L14" t="s">
+        <v>160</v>
+      </c>
+      <c r="M14" t="s">
+        <v>157</v>
+      </c>
+      <c r="N14">
+        <v>26</v>
+      </c>
+      <c r="O14" t="s">
+        <v>39</v>
+      </c>
+      <c r="P14">
+        <v>3944</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18">
+      <c r="A15" t="s">
+        <v>69</v>
+      </c>
+      <c r="B15">
+        <v>0</v>
+      </c>
+      <c r="E15" t="s">
+        <v>53</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15" t="s">
+        <v>26</v>
+      </c>
+      <c r="H15" t="s">
+        <v>26</v>
+      </c>
+      <c r="I15" t="s">
+        <v>4</v>
+      </c>
+      <c r="J15" t="s">
+        <v>74</v>
+      </c>
+      <c r="K15" t="s">
+        <v>75</v>
+      </c>
+      <c r="L15" t="s">
+        <v>76</v>
+      </c>
+      <c r="M15" t="s">
+        <v>67</v>
+      </c>
+      <c r="N15">
+        <v>18</v>
+      </c>
+      <c r="O15" t="s">
+        <v>70</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18">
+      <c r="A16" t="s">
+        <v>69</v>
+      </c>
+      <c r="B16" t="s">
+        <v>20</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16" t="s">
+        <v>19</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="G16" t="s">
+        <v>26</v>
+      </c>
+      <c r="H16" t="s">
+        <v>26</v>
+      </c>
+      <c r="I16" t="s">
+        <v>4</v>
+      </c>
+      <c r="J16" t="s">
+        <v>81</v>
+      </c>
+      <c r="K16" t="s">
+        <v>82</v>
+      </c>
+      <c r="L16" t="s">
+        <v>83</v>
+      </c>
+      <c r="M16" t="s">
+        <v>84</v>
+      </c>
+      <c r="N16">
+        <v>18</v>
+      </c>
+      <c r="O16" t="s">
+        <v>70</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17">
+      <c r="A17" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17" t="s">
+        <v>26</v>
+      </c>
+      <c r="D17" t="s">
+        <v>26</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+      <c r="G17" t="s">
+        <v>26</v>
+      </c>
+      <c r="H17" t="s">
         <v>23</v>
       </c>
-      <c r="J14" t="s">
+      <c r="I17" t="s">
         <v>4</v>
       </c>
-      <c r="K14" t="s">
+      <c r="J17" t="s">
         <v>85</v>
       </c>
-      <c r="L14" t="s">
+      <c r="K17" t="s">
         <v>86</v>
       </c>
-      <c r="M14" t="s">
+      <c r="L17" t="s">
         <v>87</v>
       </c>
-      <c r="N14" t="s">
+      <c r="M17" t="s">
         <v>88</v>
       </c>
-      <c r="O14">
-        <v>26</v>
-      </c>
-      <c r="P14" t="s">
+      <c r="N17">
+        <v>26</v>
+      </c>
+      <c r="O17" t="s">
         <v>39</v>
       </c>
-      <c r="R14" t="s">
+      <c r="Q17" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
+    <row r="18" spans="1:17">
+      <c r="A18" t="s">
         <v>18</v>
       </c>
-      <c r="J15" t="s">
+      <c r="I18" t="s">
         <v>94</v>
       </c>
-      <c r="K15">
+      <c r="J18">
         <v>1</v>
       </c>
-      <c r="L15" t="s">
+      <c r="K18" t="s">
         <v>96</v>
       </c>
-      <c r="M15" t="s">
+      <c r="L18" t="s">
         <v>97</v>
       </c>
-      <c r="N15" t="s">
+      <c r="M18" t="s">
         <v>98</v>
       </c>
-      <c r="O15">
-        <v>26</v>
-      </c>
-      <c r="P15" t="s">
+      <c r="N18">
+        <v>26</v>
+      </c>
+      <c r="O18" t="s">
         <v>39</v>
       </c>
-      <c r="R15" t="s">
+      <c r="Q18" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
+    <row r="19" spans="1:17">
+      <c r="A19" t="s">
         <v>18</v>
       </c>
-      <c r="J16" t="s">
+      <c r="I19" t="s">
         <v>106</v>
       </c>
-      <c r="K16" t="s">
+      <c r="J19" t="s">
         <v>107</v>
       </c>
-      <c r="L16" t="s">
+      <c r="K19" t="s">
         <v>108</v>
       </c>
-      <c r="M16" t="s">
+      <c r="L19" t="s">
         <v>109</v>
       </c>
-      <c r="N16" t="s">
+      <c r="M19" t="s">
         <v>110</v>
       </c>
-      <c r="O16">
-        <v>26</v>
-      </c>
-      <c r="P16" t="s">
+      <c r="N19">
+        <v>26</v>
+      </c>
+      <c r="O19" t="s">
         <v>39</v>
       </c>
-      <c r="Q16">
+      <c r="P19">
         <v>14002</v>
       </c>
-      <c r="R16" t="s">
+      <c r="Q19" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:15">
       <c r="A38" s="1" t="s">
         <v>16</v>
       </c>
@@ -1759,7 +2014,7 @@
       <c r="M38" s="1"/>
       <c r="N38" s="1"/>
     </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:15">
       <c r="A39" s="1" t="s">
         <v>0</v>
       </c>
@@ -1806,7 +2061,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:15">
       <c r="A40" t="s">
         <v>18</v>
       </c>
@@ -1850,7 +2105,7 @@
         <v>72.700999999999993</v>
       </c>
     </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:15">
       <c r="A41" t="s">
         <v>18</v>
       </c>
@@ -1888,7 +2143,7 @@
         <v>5.0039999999999996</v>
       </c>
     </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:15">
       <c r="A42" t="s">
         <v>68</v>
       </c>
@@ -1896,7 +2151,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:15">
       <c r="A43" t="s">
         <v>69</v>
       </c>
@@ -1940,7 +2195,7 @@
         <v>262.065</v>
       </c>
     </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:15">
       <c r="A44" t="s">
         <v>69</v>
       </c>
@@ -1978,7 +2233,7 @@
         <v>1162680</v>
       </c>
     </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:15">
       <c r="A45" t="s">
         <v>95</v>
       </c>
@@ -1986,7 +2241,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:15">
       <c r="A46" t="s">
         <v>18</v>
       </c>
@@ -2015,7 +2270,7 @@
         <v>9931</v>
       </c>
     </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:15">
       <c r="A47" t="s">
         <v>18</v>
       </c>
@@ -2044,7 +2299,7 @@
         <v>9856</v>
       </c>
     </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:15">
       <c r="A48" t="s">
         <v>18</v>
       </c>
@@ -2082,7 +2337,7 @@
         <v>1.6639999999999999</v>
       </c>
     </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:15">
       <c r="A49" t="s">
         <v>18</v>
       </c>
@@ -2117,7 +2372,7 @@
         <v>37.241999999999997</v>
       </c>
     </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:15">
       <c r="A54" s="1" t="s">
         <v>27</v>
       </c>
@@ -2133,7 +2388,7 @@
       <c r="K54" s="1"/>
       <c r="L54" s="1"/>
     </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:15">
       <c r="A55" s="1" t="s">
         <v>0</v>
       </c>
@@ -2172,7 +2427,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:15">
       <c r="A56" t="s">
         <v>18</v>
       </c>
@@ -2207,7 +2462,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:15">
       <c r="A57" t="s">
         <v>18</v>
       </c>
@@ -2245,7 +2500,7 @@
         <v>5590</v>
       </c>
     </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:15">
       <c r="A58" t="s">
         <v>18</v>
       </c>
@@ -2283,7 +2538,7 @@
         <v>6912</v>
       </c>
     </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:15">
       <c r="A59" t="s">
         <v>18</v>
       </c>

</xml_diff>

<commit_message>
Revert "update the FIFA_EU experimentation"
This reverts commit 555d97cfed807c48f417bc1334131f53660ecf4d.
</commit_message>
<xml_diff>
--- a/IdentityResolutionExperimentation/identity_resolution_results.xlsx
+++ b/IdentityResolutionExperimentation/identity_resolution_results.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10908"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\linar\OneDrive\Документы\GitHub\WDI_2019\IdentityResolutionExperimentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maida/Documents/GitHub/WDI_2019/IdentityResolutionExperimentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEBBE62A-3771-49E5-A375-40ED74B53410}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB4CEEDD-CB56-D444-9B97-EC6AB1C24203}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1020" yWindow="2450" windowWidth="14400" windowHeight="7360" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3200" yWindow="460" windowWidth="25600" windowHeight="16420" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blatt2" sheetId="2" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="143">
   <si>
     <t>Blocker</t>
   </si>
@@ -454,70 +454,13 @@
   </si>
   <si>
     <t>2 Minutes 22 Seconds</t>
-  </si>
-  <si>
-    <t>0.81</t>
-  </si>
-  <si>
-    <t xml:space="preserve">many false correspondences, since the first letter of the  name is the same, the DoB, height and weight are also pretty similar </t>
-  </si>
-  <si>
-    <t>deleting the MaxTokenize - worse, since the similarity for the false correspondences increased</t>
-  </si>
-  <si>
-    <t>0.9253</t>
-  </si>
-  <si>
-    <t>0.8342</t>
-  </si>
-  <si>
-    <t>0.8774</t>
-  </si>
-  <si>
-    <t>1 Minute 18 Seconds</t>
-  </si>
-  <si>
-    <t>0.67</t>
-  </si>
-  <si>
-    <t>decreasing the threshold gave more true correspondences</t>
-  </si>
-  <si>
-    <t>there is some false correspondences, maybe increase the treshold</t>
-  </si>
-  <si>
-    <t>there is some false correspondences, so increase the threshold</t>
-  </si>
-  <si>
-    <t>0.9693</t>
-  </si>
-  <si>
-    <t>0.8187</t>
-  </si>
-  <si>
-    <t>0.8876</t>
-  </si>
-  <si>
-    <t>2 Minutes 33 Seconds</t>
-  </si>
-  <si>
-    <t>0.76</t>
-  </si>
-  <si>
-    <t>0.8031</t>
-  </si>
-  <si>
-    <t>0.8782</t>
-  </si>
-  <si>
-    <t>0.78</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -660,75 +603,75 @@
     </xf>
   </cellXfs>
   <cellStyles count="69">
-    <cellStyle name="Гиперссылка" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Гиперссылка" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Гиперссылка" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="Гиперссылка" xfId="7" builtinId="8" hidden="1"/>
-    <cellStyle name="Гиперссылка" xfId="9" builtinId="8" hidden="1"/>
-    <cellStyle name="Гиперссылка" xfId="11" builtinId="8" hidden="1"/>
-    <cellStyle name="Гиперссылка" xfId="13" builtinId="8" hidden="1"/>
-    <cellStyle name="Гиперссылка" xfId="15" builtinId="8" hidden="1"/>
-    <cellStyle name="Гиперссылка" xfId="17" builtinId="8" hidden="1"/>
-    <cellStyle name="Гиперссылка" xfId="19" builtinId="8" hidden="1"/>
-    <cellStyle name="Гиперссылка" xfId="21" builtinId="8" hidden="1"/>
-    <cellStyle name="Гиперссылка" xfId="23" builtinId="8" hidden="1"/>
-    <cellStyle name="Гиперссылка" xfId="25" builtinId="8" hidden="1"/>
-    <cellStyle name="Гиперссылка" xfId="27" builtinId="8" hidden="1"/>
-    <cellStyle name="Гиперссылка" xfId="29" builtinId="8" hidden="1"/>
-    <cellStyle name="Гиперссылка" xfId="31" builtinId="8" hidden="1"/>
-    <cellStyle name="Гиперссылка" xfId="33" builtinId="8" hidden="1"/>
-    <cellStyle name="Гиперссылка" xfId="35" builtinId="8" hidden="1"/>
-    <cellStyle name="Гиперссылка" xfId="37" builtinId="8" hidden="1"/>
-    <cellStyle name="Гиперссылка" xfId="39" builtinId="8" hidden="1"/>
-    <cellStyle name="Гиперссылка" xfId="41" builtinId="8" hidden="1"/>
-    <cellStyle name="Гиперссылка" xfId="43" builtinId="8" hidden="1"/>
-    <cellStyle name="Гиперссылка" xfId="45" builtinId="8" hidden="1"/>
-    <cellStyle name="Гиперссылка" xfId="47" builtinId="8" hidden="1"/>
-    <cellStyle name="Гиперссылка" xfId="49" builtinId="8" hidden="1"/>
-    <cellStyle name="Гиперссылка" xfId="51" builtinId="8" hidden="1"/>
-    <cellStyle name="Гиперссылка" xfId="53" builtinId="8" hidden="1"/>
-    <cellStyle name="Гиперссылка" xfId="55" builtinId="8" hidden="1"/>
-    <cellStyle name="Гиперссылка" xfId="57" builtinId="8" hidden="1"/>
-    <cellStyle name="Гиперссылка" xfId="59" builtinId="8" hidden="1"/>
-    <cellStyle name="Гиперссылка" xfId="61" builtinId="8" hidden="1"/>
-    <cellStyle name="Гиперссылка" xfId="63" builtinId="8" hidden="1"/>
-    <cellStyle name="Гиперссылка" xfId="65" builtinId="8" hidden="1"/>
-    <cellStyle name="Гиперссылка" xfId="67" builtinId="8" hidden="1"/>
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
-    <cellStyle name="Открывавшаяся гиперссылка" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Открывавшаяся гиперссылка" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Открывавшаяся гиперссылка" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Открывавшаяся гиперссылка" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Открывавшаяся гиперссылка" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Открывавшаяся гиперссылка" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="Открывавшаяся гиперссылка" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="Открывавшаяся гиперссылка" xfId="16" builtinId="9" hidden="1"/>
-    <cellStyle name="Открывавшаяся гиперссылка" xfId="18" builtinId="9" hidden="1"/>
-    <cellStyle name="Открывавшаяся гиперссылка" xfId="20" builtinId="9" hidden="1"/>
-    <cellStyle name="Открывавшаяся гиперссылка" xfId="22" builtinId="9" hidden="1"/>
-    <cellStyle name="Открывавшаяся гиперссылка" xfId="24" builtinId="9" hidden="1"/>
-    <cellStyle name="Открывавшаяся гиперссылка" xfId="26" builtinId="9" hidden="1"/>
-    <cellStyle name="Открывавшаяся гиперссылка" xfId="28" builtinId="9" hidden="1"/>
-    <cellStyle name="Открывавшаяся гиперссылка" xfId="30" builtinId="9" hidden="1"/>
-    <cellStyle name="Открывавшаяся гиперссылка" xfId="32" builtinId="9" hidden="1"/>
-    <cellStyle name="Открывавшаяся гиперссылка" xfId="34" builtinId="9" hidden="1"/>
-    <cellStyle name="Открывавшаяся гиперссылка" xfId="36" builtinId="9" hidden="1"/>
-    <cellStyle name="Открывавшаяся гиперссылка" xfId="38" builtinId="9" hidden="1"/>
-    <cellStyle name="Открывавшаяся гиперссылка" xfId="40" builtinId="9" hidden="1"/>
-    <cellStyle name="Открывавшаяся гиперссылка" xfId="42" builtinId="9" hidden="1"/>
-    <cellStyle name="Открывавшаяся гиперссылка" xfId="44" builtinId="9" hidden="1"/>
-    <cellStyle name="Открывавшаяся гиперссылка" xfId="46" builtinId="9" hidden="1"/>
-    <cellStyle name="Открывавшаяся гиперссылка" xfId="48" builtinId="9" hidden="1"/>
-    <cellStyle name="Открывавшаяся гиперссылка" xfId="50" builtinId="9" hidden="1"/>
-    <cellStyle name="Открывавшаяся гиперссылка" xfId="52" builtinId="9" hidden="1"/>
-    <cellStyle name="Открывавшаяся гиперссылка" xfId="54" builtinId="9" hidden="1"/>
-    <cellStyle name="Открывавшаяся гиперссылка" xfId="56" builtinId="9" hidden="1"/>
-    <cellStyle name="Открывавшаяся гиперссылка" xfId="58" builtinId="9" hidden="1"/>
-    <cellStyle name="Открывавшаяся гиперссылка" xfId="60" builtinId="9" hidden="1"/>
-    <cellStyle name="Открывавшаяся гиперссылка" xfId="62" builtinId="9" hidden="1"/>
-    <cellStyle name="Открывавшаяся гиперссылка" xfId="64" builtinId="9" hidden="1"/>
-    <cellStyle name="Открывавшаяся гиперссылка" xfId="66" builtinId="9" hidden="1"/>
-    <cellStyle name="Открывавшаяся гиперссылка" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -1067,11 +1010,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K7" zoomScale="75" workbookViewId="0">
-      <selection activeCell="U16" sqref="U16"/>
+    <sheetView tabSelected="1" topLeftCell="E33" zoomScale="75" workbookViewId="0">
+      <selection activeCell="O41" sqref="O41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="44.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="44.33203125" customWidth="1"/>
@@ -1089,288 +1032,270 @@
     <col min="16" max="16" width="14.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B1" s="1"/>
     </row>
-    <row r="2" spans="1:18">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="1"/>
+      <c r="C2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="K2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="L2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="M2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="N2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="O2" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="O2" s="1" t="s">
+      <c r="P2" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="P2" s="1" t="s">
+      <c r="Q2" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="Q2" s="1" t="s">
+      <c r="R2" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="R2" s="1"/>
-    </row>
-    <row r="3" spans="1:18">
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>5</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>20</v>
       </c>
-      <c r="C3">
-        <v>0</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3" t="s">
         <v>19</v>
       </c>
-      <c r="E3">
-        <v>0</v>
-      </c>
       <c r="F3">
         <v>0</v>
       </c>
-      <c r="G3" t="s">
-        <v>26</v>
+      <c r="G3">
+        <v>0</v>
       </c>
       <c r="H3" t="s">
         <v>26</v>
       </c>
       <c r="I3" t="s">
+        <v>26</v>
+      </c>
+      <c r="J3" t="s">
         <v>4</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>21</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
         <v>22</v>
       </c>
-      <c r="L3" t="s">
+      <c r="M3" t="s">
         <v>23</v>
       </c>
-      <c r="M3" t="s">
+      <c r="N3" t="s">
         <v>24</v>
       </c>
-      <c r="N3">
+      <c r="O3">
         <v>6</v>
       </c>
-      <c r="O3" t="s">
-        <v>143</v>
-      </c>
-      <c r="P3">
-        <v>18246</v>
-      </c>
-      <c r="Q3" t="s">
+      <c r="R3" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:18">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>34</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>20</v>
       </c>
-      <c r="C4">
-        <v>0</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4" t="s">
         <v>19</v>
       </c>
-      <c r="E4">
-        <v>0</v>
-      </c>
       <c r="F4">
         <v>0</v>
       </c>
-      <c r="G4" t="s">
-        <v>26</v>
+      <c r="G4">
+        <v>0</v>
       </c>
       <c r="H4" t="s">
         <v>26</v>
       </c>
       <c r="I4" t="s">
+        <v>26</v>
+      </c>
+      <c r="J4" t="s">
         <v>4</v>
       </c>
-      <c r="J4">
+      <c r="K4">
         <v>1</v>
       </c>
-      <c r="K4" t="s">
+      <c r="L4" t="s">
         <v>35</v>
       </c>
-      <c r="L4" t="s">
+      <c r="M4" t="s">
         <v>36</v>
       </c>
-      <c r="M4" t="s">
+      <c r="N4" t="s">
         <v>40</v>
       </c>
-      <c r="N4">
+      <c r="O4">
         <v>7</v>
       </c>
-      <c r="O4" t="s">
+      <c r="P4" t="s">
         <v>38</v>
       </c>
-      <c r="P4">
-        <v>437</v>
-      </c>
-      <c r="Q4" t="s">
+      <c r="R4" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:18">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>18</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>20</v>
       </c>
-      <c r="C5">
-        <v>0</v>
-      </c>
-      <c r="D5" t="s">
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5" t="s">
         <v>19</v>
       </c>
-      <c r="E5">
-        <v>0</v>
-      </c>
       <c r="F5">
         <v>0</v>
       </c>
-      <c r="G5" t="s">
-        <v>26</v>
+      <c r="G5">
+        <v>0</v>
       </c>
       <c r="H5" t="s">
         <v>26</v>
       </c>
       <c r="I5" t="s">
+        <v>26</v>
+      </c>
+      <c r="J5" t="s">
         <v>4</v>
       </c>
-      <c r="J5" t="s">
+      <c r="K5" t="s">
         <v>43</v>
       </c>
-      <c r="K5" t="s">
+      <c r="L5" t="s">
         <v>44</v>
       </c>
-      <c r="L5" t="s">
+      <c r="M5" t="s">
         <v>45</v>
       </c>
-      <c r="M5" t="s">
+      <c r="N5" t="s">
         <v>42</v>
       </c>
-      <c r="N5">
-        <v>26</v>
-      </c>
-      <c r="O5" t="s">
+      <c r="O5">
+        <v>26</v>
+      </c>
+      <c r="P5" t="s">
         <v>39</v>
       </c>
-      <c r="P5">
-        <v>18019</v>
-      </c>
-      <c r="Q5" t="s">
+      <c r="R5" t="s">
         <v>29</v>
       </c>
-      <c r="R5" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="6" spans="1:18">
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>46</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>20</v>
       </c>
-      <c r="C6">
-        <v>0</v>
-      </c>
-      <c r="D6" t="s">
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6" t="s">
         <v>19</v>
       </c>
-      <c r="E6">
-        <v>0</v>
-      </c>
       <c r="F6">
         <v>0</v>
       </c>
-      <c r="G6" t="s">
-        <v>26</v>
+      <c r="G6">
+        <v>0</v>
       </c>
       <c r="H6" t="s">
         <v>26</v>
       </c>
       <c r="I6" t="s">
+        <v>26</v>
+      </c>
+      <c r="J6" t="s">
         <v>4</v>
       </c>
-      <c r="J6" t="s">
+      <c r="K6" t="s">
         <v>47</v>
       </c>
-      <c r="K6" t="s">
+      <c r="L6" t="s">
         <v>48</v>
       </c>
-      <c r="L6" t="s">
+      <c r="M6" t="s">
         <v>49</v>
       </c>
-      <c r="M6" t="s">
+      <c r="N6" t="s">
         <v>50</v>
       </c>
-      <c r="N6">
+      <c r="O6">
         <v>7</v>
       </c>
-      <c r="O6" t="s">
+      <c r="P6" t="s">
         <v>51</v>
       </c>
-      <c r="Q6" t="s">
+      <c r="R6" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:18">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>18</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>53</v>
       </c>
-      <c r="C7">
-        <v>0</v>
-      </c>
       <c r="D7">
         <v>0</v>
       </c>
@@ -1380,50 +1305,44 @@
       <c r="F7">
         <v>0</v>
       </c>
-      <c r="G7" t="s">
-        <v>26</v>
+      <c r="G7">
+        <v>0</v>
       </c>
       <c r="H7" t="s">
         <v>26</v>
       </c>
       <c r="I7" t="s">
+        <v>26</v>
+      </c>
+      <c r="J7" t="s">
         <v>4</v>
       </c>
-      <c r="J7" t="s">
+      <c r="K7" t="s">
         <v>54</v>
       </c>
-      <c r="K7" t="s">
+      <c r="L7" t="s">
         <v>55</v>
       </c>
-      <c r="L7" t="s">
+      <c r="M7" t="s">
         <v>56</v>
       </c>
-      <c r="M7" t="s">
+      <c r="N7" t="s">
         <v>52</v>
       </c>
-      <c r="N7">
-        <v>26</v>
-      </c>
-      <c r="O7" t="s">
+      <c r="O7">
+        <v>26</v>
+      </c>
+      <c r="P7" t="s">
         <v>39</v>
       </c>
-      <c r="P7">
-        <v>11468</v>
-      </c>
-      <c r="Q7" t="s">
+      <c r="R7" t="s">
         <v>29</v>
       </c>
-      <c r="R7" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="8" spans="1:18">
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>18</v>
       </c>
-      <c r="B8">
-        <v>0</v>
-      </c>
       <c r="C8">
         <v>0</v>
       </c>
@@ -1433,570 +1352,396 @@
       <c r="E8">
         <v>0</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8" t="s">
         <v>53</v>
       </c>
-      <c r="G8" t="s">
-        <v>26</v>
-      </c>
       <c r="H8" t="s">
         <v>26</v>
       </c>
       <c r="I8" t="s">
+        <v>26</v>
+      </c>
+      <c r="J8" t="s">
         <v>4</v>
       </c>
-      <c r="J8" t="s">
+      <c r="K8" t="s">
         <v>57</v>
       </c>
-      <c r="K8" t="s">
+      <c r="L8" t="s">
         <v>58</v>
       </c>
-      <c r="L8" t="s">
+      <c r="M8" t="s">
         <v>59</v>
       </c>
-      <c r="M8" t="s">
+      <c r="N8" t="s">
         <v>60</v>
       </c>
-      <c r="N8">
-        <v>26</v>
-      </c>
-      <c r="O8" t="s">
+      <c r="O8">
+        <v>26</v>
+      </c>
+      <c r="P8" t="s">
         <v>39</v>
       </c>
-      <c r="P8">
-        <v>4010</v>
-      </c>
-      <c r="Q8" t="s">
+      <c r="R8" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:18">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>18</v>
       </c>
-      <c r="B9">
-        <v>0</v>
-      </c>
-      <c r="C9">
-        <v>0</v>
+      <c r="C9" t="s">
+        <v>19</v>
       </c>
       <c r="D9">
         <v>0</v>
       </c>
-      <c r="E9">
-        <v>0</v>
-      </c>
-      <c r="F9" t="s">
+      <c r="E9" t="s">
+        <v>19</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9" t="s">
+        <v>61</v>
+      </c>
+      <c r="I9" t="s">
         <v>53</v>
       </c>
-      <c r="G9" t="s">
-        <v>26</v>
-      </c>
-      <c r="H9" t="s">
-        <v>26</v>
-      </c>
-      <c r="I9" t="s">
+      <c r="J9" t="s">
         <v>4</v>
       </c>
-      <c r="J9" t="s">
-        <v>146</v>
-      </c>
       <c r="K9" t="s">
-        <v>147</v>
+        <v>66</v>
       </c>
       <c r="L9" t="s">
-        <v>148</v>
+        <v>55</v>
       </c>
       <c r="M9" t="s">
-        <v>149</v>
-      </c>
-      <c r="N9">
-        <v>26</v>
-      </c>
-      <c r="O9" t="s">
+        <v>30</v>
+      </c>
+      <c r="N9" t="s">
+        <v>67</v>
+      </c>
+      <c r="O9">
+        <v>26</v>
+      </c>
+      <c r="P9" t="s">
         <v>39</v>
       </c>
-      <c r="P9">
-        <v>4238</v>
-      </c>
-      <c r="Q9" t="s">
-        <v>150</v>
-      </c>
       <c r="R9" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="10" spans="1:18">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>18</v>
       </c>
-      <c r="B10" t="s">
-        <v>19</v>
-      </c>
       <c r="C10">
         <v>0</v>
       </c>
-      <c r="D10" t="s">
-        <v>19</v>
+      <c r="D10">
+        <v>0</v>
       </c>
       <c r="E10">
         <v>0</v>
       </c>
-      <c r="F10">
-        <v>0</v>
-      </c>
-      <c r="G10" t="s">
-        <v>61</v>
+      <c r="F10" t="s">
+        <v>53</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
       </c>
       <c r="H10" t="s">
-        <v>53</v>
+        <v>26</v>
       </c>
       <c r="I10" t="s">
+        <v>26</v>
+      </c>
+      <c r="J10" t="s">
         <v>4</v>
       </c>
-      <c r="J10" t="s">
-        <v>66</v>
-      </c>
       <c r="K10" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
       <c r="L10" t="s">
-        <v>30</v>
+        <v>73</v>
       </c>
       <c r="M10" t="s">
-        <v>67</v>
-      </c>
-      <c r="N10">
-        <v>26</v>
-      </c>
-      <c r="O10" t="s">
+        <v>63</v>
+      </c>
+      <c r="N10" t="s">
+        <v>64</v>
+      </c>
+      <c r="O10">
+        <v>26</v>
+      </c>
+      <c r="P10" t="s">
         <v>39</v>
       </c>
-      <c r="Q10" t="s">
+      <c r="R10" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:18">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>18</v>
       </c>
-      <c r="B11">
-        <v>0</v>
-      </c>
-      <c r="C11">
-        <v>0</v>
+      <c r="C11" t="s">
+        <v>26</v>
       </c>
       <c r="D11">
         <v>0</v>
       </c>
       <c r="E11" t="s">
+        <v>26</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11" t="s">
+        <v>26</v>
+      </c>
+      <c r="I11" t="s">
+        <v>26</v>
+      </c>
+      <c r="J11" t="s">
+        <v>4</v>
+      </c>
+      <c r="K11" t="s">
+        <v>72</v>
+      </c>
+      <c r="L11" t="s">
+        <v>77</v>
+      </c>
+      <c r="M11" t="s">
+        <v>78</v>
+      </c>
+      <c r="N11" t="s">
+        <v>80</v>
+      </c>
+      <c r="O11">
+        <v>26</v>
+      </c>
+      <c r="P11" t="s">
+        <v>39</v>
+      </c>
+      <c r="R11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>69</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="F12" t="s">
         <v>53</v>
       </c>
-      <c r="F11">
-        <v>0</v>
-      </c>
-      <c r="G11" t="s">
-        <v>26</v>
-      </c>
-      <c r="H11" t="s">
-        <v>26</v>
-      </c>
-      <c r="I11" t="s">
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12" t="s">
+        <v>26</v>
+      </c>
+      <c r="I12" t="s">
+        <v>26</v>
+      </c>
+      <c r="J12" t="s">
         <v>4</v>
       </c>
-      <c r="J11" t="s">
-        <v>62</v>
-      </c>
-      <c r="K11" t="s">
-        <v>73</v>
-      </c>
-      <c r="L11" t="s">
-        <v>63</v>
-      </c>
-      <c r="M11" t="s">
-        <v>64</v>
-      </c>
-      <c r="N11">
-        <v>26</v>
-      </c>
-      <c r="O11" t="s">
-        <v>39</v>
-      </c>
-      <c r="P11">
-        <v>4199</v>
-      </c>
-      <c r="Q11" t="s">
+      <c r="K12" t="s">
+        <v>74</v>
+      </c>
+      <c r="L12" t="s">
+        <v>75</v>
+      </c>
+      <c r="M12" t="s">
+        <v>76</v>
+      </c>
+      <c r="N12" t="s">
+        <v>67</v>
+      </c>
+      <c r="O12">
+        <v>18</v>
+      </c>
+      <c r="P12" t="s">
+        <v>70</v>
+      </c>
+      <c r="R12" t="s">
         <v>29</v>
       </c>
-      <c r="R11" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="12" spans="1:18">
-      <c r="A12" t="s">
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>69</v>
+      </c>
+      <c r="C13" t="s">
+        <v>20</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13" t="s">
+        <v>19</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13" t="s">
+        <v>26</v>
+      </c>
+      <c r="I13" t="s">
+        <v>26</v>
+      </c>
+      <c r="J13" t="s">
+        <v>4</v>
+      </c>
+      <c r="K13" t="s">
+        <v>81</v>
+      </c>
+      <c r="L13" t="s">
+        <v>82</v>
+      </c>
+      <c r="M13" t="s">
+        <v>83</v>
+      </c>
+      <c r="N13" t="s">
+        <v>84</v>
+      </c>
+      <c r="O13">
         <v>18</v>
       </c>
-      <c r="B12" t="s">
-        <v>26</v>
-      </c>
-      <c r="C12">
-        <v>0</v>
-      </c>
-      <c r="D12" t="s">
-        <v>26</v>
-      </c>
-      <c r="E12">
-        <v>0</v>
-      </c>
-      <c r="F12">
-        <v>0</v>
-      </c>
-      <c r="G12" t="s">
-        <v>26</v>
-      </c>
-      <c r="H12" t="s">
-        <v>26</v>
-      </c>
-      <c r="I12" t="s">
-        <v>4</v>
-      </c>
-      <c r="J12" t="s">
-        <v>72</v>
-      </c>
-      <c r="K12" t="s">
-        <v>77</v>
-      </c>
-      <c r="L12" t="s">
-        <v>78</v>
-      </c>
-      <c r="M12" t="s">
-        <v>80</v>
-      </c>
-      <c r="N12">
-        <v>26</v>
-      </c>
-      <c r="O12" t="s">
-        <v>39</v>
-      </c>
-      <c r="P12">
-        <v>21468</v>
-      </c>
-      <c r="Q12" t="s">
+      <c r="P13" t="s">
+        <v>70</v>
+      </c>
+      <c r="R13" t="s">
         <v>29</v>
       </c>
-      <c r="R12" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="13" spans="1:18">
-      <c r="A13" t="s">
-        <v>18</v>
-      </c>
-      <c r="B13" t="s">
-        <v>26</v>
-      </c>
-      <c r="C13">
-        <v>0</v>
-      </c>
-      <c r="D13" t="s">
-        <v>26</v>
-      </c>
-      <c r="E13">
-        <v>0</v>
-      </c>
-      <c r="F13">
-        <v>0</v>
-      </c>
-      <c r="G13" t="s">
-        <v>26</v>
-      </c>
-      <c r="H13" t="s">
-        <v>26</v>
-      </c>
-      <c r="I13" t="s">
-        <v>4</v>
-      </c>
-      <c r="J13" t="s">
-        <v>154</v>
-      </c>
-      <c r="K13" t="s">
-        <v>155</v>
-      </c>
-      <c r="L13" t="s">
-        <v>156</v>
-      </c>
-      <c r="M13" t="s">
-        <v>157</v>
-      </c>
-      <c r="N13">
-        <v>26</v>
-      </c>
-      <c r="O13" t="s">
-        <v>39</v>
-      </c>
-      <c r="P13">
-        <v>4546</v>
-      </c>
-      <c r="Q13" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="14" spans="1:18">
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>18</v>
       </c>
-      <c r="B14" t="s">
-        <v>26</v>
-      </c>
-      <c r="C14">
-        <v>0</v>
-      </c>
-      <c r="D14" t="s">
-        <v>26</v>
-      </c>
-      <c r="E14">
-        <v>0</v>
+      <c r="C14" t="s">
+        <v>26</v>
+      </c>
+      <c r="E14" t="s">
+        <v>26</v>
       </c>
       <c r="F14">
         <v>0</v>
       </c>
-      <c r="G14" t="s">
-        <v>26</v>
+      <c r="G14">
+        <v>0</v>
       </c>
       <c r="H14" t="s">
         <v>26</v>
       </c>
       <c r="I14" t="s">
+        <v>23</v>
+      </c>
+      <c r="J14" t="s">
         <v>4</v>
       </c>
-      <c r="J14" t="s">
-        <v>131</v>
-      </c>
       <c r="K14" t="s">
-        <v>159</v>
+        <v>85</v>
       </c>
       <c r="L14" t="s">
-        <v>160</v>
+        <v>86</v>
       </c>
       <c r="M14" t="s">
-        <v>157</v>
-      </c>
-      <c r="N14">
-        <v>26</v>
-      </c>
-      <c r="O14" t="s">
+        <v>87</v>
+      </c>
+      <c r="N14" t="s">
+        <v>88</v>
+      </c>
+      <c r="O14">
+        <v>26</v>
+      </c>
+      <c r="P14" t="s">
         <v>39</v>
       </c>
-      <c r="P14">
-        <v>3944</v>
-      </c>
-      <c r="Q14" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="15" spans="1:18">
+      <c r="R14" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>69</v>
-      </c>
-      <c r="B15">
-        <v>0</v>
-      </c>
-      <c r="E15" t="s">
-        <v>53</v>
-      </c>
-      <c r="F15">
-        <v>0</v>
-      </c>
-      <c r="G15" t="s">
-        <v>26</v>
-      </c>
-      <c r="H15" t="s">
-        <v>26</v>
-      </c>
-      <c r="I15" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="J15" t="s">
-        <v>74</v>
-      </c>
-      <c r="K15" t="s">
-        <v>75</v>
+        <v>94</v>
+      </c>
+      <c r="K15">
+        <v>1</v>
       </c>
       <c r="L15" t="s">
-        <v>76</v>
+        <v>96</v>
       </c>
       <c r="M15" t="s">
-        <v>67</v>
-      </c>
-      <c r="N15">
+        <v>97</v>
+      </c>
+      <c r="N15" t="s">
+        <v>98</v>
+      </c>
+      <c r="O15">
+        <v>26</v>
+      </c>
+      <c r="P15" t="s">
+        <v>39</v>
+      </c>
+      <c r="R15" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
         <v>18</v>
       </c>
-      <c r="O15" t="s">
-        <v>70</v>
-      </c>
-      <c r="Q15" t="s">
+      <c r="J16" t="s">
+        <v>106</v>
+      </c>
+      <c r="K16" t="s">
+        <v>107</v>
+      </c>
+      <c r="L16" t="s">
+        <v>108</v>
+      </c>
+      <c r="M16" t="s">
+        <v>109</v>
+      </c>
+      <c r="N16" t="s">
+        <v>110</v>
+      </c>
+      <c r="O16">
+        <v>26</v>
+      </c>
+      <c r="P16" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q16">
+        <v>14002</v>
+      </c>
+      <c r="R16" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="1:18">
-      <c r="A16" t="s">
-        <v>69</v>
-      </c>
-      <c r="B16" t="s">
-        <v>20</v>
-      </c>
-      <c r="C16">
-        <v>0</v>
-      </c>
-      <c r="D16" t="s">
-        <v>19</v>
-      </c>
-      <c r="E16">
-        <v>0</v>
-      </c>
-      <c r="F16">
-        <v>0</v>
-      </c>
-      <c r="G16" t="s">
-        <v>26</v>
-      </c>
-      <c r="H16" t="s">
-        <v>26</v>
-      </c>
-      <c r="I16" t="s">
-        <v>4</v>
-      </c>
-      <c r="J16" t="s">
-        <v>81</v>
-      </c>
-      <c r="K16" t="s">
-        <v>82</v>
-      </c>
-      <c r="L16" t="s">
-        <v>83</v>
-      </c>
-      <c r="M16" t="s">
-        <v>84</v>
-      </c>
-      <c r="N16">
-        <v>18</v>
-      </c>
-      <c r="O16" t="s">
-        <v>70</v>
-      </c>
-      <c r="Q16" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="17" spans="1:17">
-      <c r="A17" t="s">
-        <v>18</v>
-      </c>
-      <c r="B17" t="s">
-        <v>26</v>
-      </c>
-      <c r="D17" t="s">
-        <v>26</v>
-      </c>
-      <c r="E17">
-        <v>0</v>
-      </c>
-      <c r="F17">
-        <v>0</v>
-      </c>
-      <c r="G17" t="s">
-        <v>26</v>
-      </c>
-      <c r="H17" t="s">
-        <v>23</v>
-      </c>
-      <c r="I17" t="s">
-        <v>4</v>
-      </c>
-      <c r="J17" t="s">
-        <v>85</v>
-      </c>
-      <c r="K17" t="s">
-        <v>86</v>
-      </c>
-      <c r="L17" t="s">
-        <v>87</v>
-      </c>
-      <c r="M17" t="s">
-        <v>88</v>
-      </c>
-      <c r="N17">
-        <v>26</v>
-      </c>
-      <c r="O17" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q17" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="18" spans="1:17">
-      <c r="A18" t="s">
-        <v>18</v>
-      </c>
-      <c r="I18" t="s">
-        <v>94</v>
-      </c>
-      <c r="J18">
-        <v>1</v>
-      </c>
-      <c r="K18" t="s">
-        <v>96</v>
-      </c>
-      <c r="L18" t="s">
-        <v>97</v>
-      </c>
-      <c r="M18" t="s">
-        <v>98</v>
-      </c>
-      <c r="N18">
-        <v>26</v>
-      </c>
-      <c r="O18" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q18" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="19" spans="1:17">
-      <c r="A19" t="s">
-        <v>18</v>
-      </c>
-      <c r="I19" t="s">
-        <v>106</v>
-      </c>
-      <c r="J19" t="s">
-        <v>107</v>
-      </c>
-      <c r="K19" t="s">
-        <v>108</v>
-      </c>
-      <c r="L19" t="s">
-        <v>109</v>
-      </c>
-      <c r="M19" t="s">
-        <v>110</v>
-      </c>
-      <c r="N19">
-        <v>26</v>
-      </c>
-      <c r="O19" t="s">
-        <v>39</v>
-      </c>
-      <c r="P19">
-        <v>14002</v>
-      </c>
-      <c r="Q19" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="38" spans="1:15">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>16</v>
       </c>
@@ -2014,7 +1759,7 @@
       <c r="M38" s="1"/>
       <c r="N38" s="1"/>
     </row>
-    <row r="39" spans="1:15">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>0</v>
       </c>
@@ -2061,7 +1806,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="40" spans="1:15">
+    <row r="40" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>18</v>
       </c>
@@ -2105,7 +1850,7 @@
         <v>72.700999999999993</v>
       </c>
     </row>
-    <row r="41" spans="1:15">
+    <row r="41" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>18</v>
       </c>
@@ -2143,7 +1888,7 @@
         <v>5.0039999999999996</v>
       </c>
     </row>
-    <row r="42" spans="1:15">
+    <row r="42" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>68</v>
       </c>
@@ -2151,7 +1896,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="43" spans="1:15">
+    <row r="43" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>69</v>
       </c>
@@ -2195,7 +1940,7 @@
         <v>262.065</v>
       </c>
     </row>
-    <row r="44" spans="1:15">
+    <row r="44" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>69</v>
       </c>
@@ -2233,7 +1978,7 @@
         <v>1162680</v>
       </c>
     </row>
-    <row r="45" spans="1:15">
+    <row r="45" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>95</v>
       </c>
@@ -2241,7 +1986,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="46" spans="1:15">
+    <row r="46" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>18</v>
       </c>
@@ -2270,7 +2015,7 @@
         <v>9931</v>
       </c>
     </row>
-    <row r="47" spans="1:15">
+    <row r="47" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>18</v>
       </c>
@@ -2299,7 +2044,7 @@
         <v>9856</v>
       </c>
     </row>
-    <row r="48" spans="1:15">
+    <row r="48" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>18</v>
       </c>
@@ -2337,7 +2082,7 @@
         <v>1.6639999999999999</v>
       </c>
     </row>
-    <row r="49" spans="1:15">
+    <row r="49" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>18</v>
       </c>
@@ -2372,7 +2117,7 @@
         <v>37.241999999999997</v>
       </c>
     </row>
-    <row r="54" spans="1:15">
+    <row r="54" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
         <v>27</v>
       </c>
@@ -2388,7 +2133,7 @@
       <c r="K54" s="1"/>
       <c r="L54" s="1"/>
     </row>
-    <row r="55" spans="1:15">
+    <row r="55" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
         <v>0</v>
       </c>
@@ -2427,7 +2172,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="56" spans="1:15">
+    <row r="56" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>18</v>
       </c>
@@ -2462,7 +2207,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="57" spans="1:15">
+    <row r="57" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>18</v>
       </c>
@@ -2500,7 +2245,7 @@
         <v>5590</v>
       </c>
     </row>
-    <row r="58" spans="1:15">
+    <row r="58" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>18</v>
       </c>
@@ -2538,7 +2283,7 @@
         <v>6912</v>
       </c>
     </row>
-    <row r="59" spans="1:15">
+    <row r="59" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>18</v>
       </c>

</xml_diff>

<commit_message>
recover api transfer identity resolution results
</commit_message>
<xml_diff>
--- a/IdentityResolutionExperimentation/identity_resolution_results.xlsx
+++ b/IdentityResolutionExperimentation/identity_resolution_results.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10908"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26621"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maida/Documents/GitHub/WDI_2019/IdentityResolutionExperimentation/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB4CEEDD-CB56-D444-9B97-EC6AB1C24203}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3200" yWindow="460" windowWidth="25600" windowHeight="16420" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Blatt2" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140000"/>
+  <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -25,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="153">
   <si>
     <t>Blocker</t>
   </si>
@@ -108,9 +102,6 @@
     <t>0.25</t>
   </si>
   <si>
-    <t>API-Transfers</t>
-  </si>
-  <si>
     <t>Name:Levenshtein</t>
   </si>
   <si>
@@ -454,12 +445,45 @@
   </si>
   <si>
     <t>2 Minutes 22 Seconds</t>
+  </si>
+  <si>
+    <t>Extra Information: sim=1 if Levenshtein =1 and and date_sim != 0</t>
+  </si>
+  <si>
+    <t>0.85</t>
+  </si>
+  <si>
+    <t>0.15</t>
+  </si>
+  <si>
+    <t>0.9519</t>
+  </si>
+  <si>
+    <t>0.7984</t>
+  </si>
+  <si>
+    <t>0.8684</t>
+  </si>
+  <si>
+    <t>2 Minutes 44 Seconds</t>
+  </si>
+  <si>
+    <t>0.9515</t>
+  </si>
+  <si>
+    <t>0.7903</t>
+  </si>
+  <si>
+    <t>0.8634</t>
+  </si>
+  <si>
+    <t>2 Minutes 25 Seconds</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -603,75 +627,75 @@
     </xf>
   </cellXfs>
   <cellStyles count="69">
-    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Besuchter Link" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Link" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -1007,14 +1031,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E33" zoomScale="75" workbookViewId="0">
-      <selection activeCell="O41" sqref="O41"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="75" workbookViewId="0">
+      <selection activeCell="C60" sqref="C60"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="44.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="44.33203125" customWidth="1"/>
@@ -1032,13 +1056,13 @@
     <col min="16" max="16" width="14.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:18">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B1" s="1"/>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:18">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1083,16 +1107,16 @@
         <v>25</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="Q2" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="R2" s="1" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -1136,12 +1160,12 @@
         <v>6</v>
       </c>
       <c r="R3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18">
       <c r="A4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C4" t="s">
         <v>20</v>
@@ -1171,25 +1195,25 @@
         <v>1</v>
       </c>
       <c r="L4" t="s">
+        <v>34</v>
+      </c>
+      <c r="M4" t="s">
         <v>35</v>
       </c>
-      <c r="M4" t="s">
-        <v>36</v>
-      </c>
       <c r="N4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="O4">
         <v>7</v>
       </c>
       <c r="P4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="R4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -1218,30 +1242,30 @@
         <v>4</v>
       </c>
       <c r="K5" t="s">
+        <v>42</v>
+      </c>
+      <c r="L5" t="s">
         <v>43</v>
       </c>
-      <c r="L5" t="s">
+      <c r="M5" t="s">
         <v>44</v>
       </c>
-      <c r="M5" t="s">
+      <c r="N5" t="s">
+        <v>41</v>
+      </c>
+      <c r="O5">
+        <v>26</v>
+      </c>
+      <c r="P5" t="s">
+        <v>38</v>
+      </c>
+      <c r="R5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18">
+      <c r="A6" t="s">
         <v>45</v>
-      </c>
-      <c r="N5" t="s">
-        <v>42</v>
-      </c>
-      <c r="O5">
-        <v>26</v>
-      </c>
-      <c r="P5" t="s">
-        <v>39</v>
-      </c>
-      <c r="R5" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>46</v>
       </c>
       <c r="C6" t="s">
         <v>20</v>
@@ -1268,33 +1292,33 @@
         <v>4</v>
       </c>
       <c r="K6" t="s">
+        <v>46</v>
+      </c>
+      <c r="L6" t="s">
         <v>47</v>
       </c>
-      <c r="L6" t="s">
+      <c r="M6" t="s">
         <v>48</v>
       </c>
-      <c r="M6" t="s">
+      <c r="N6" t="s">
         <v>49</v>
-      </c>
-      <c r="N6" t="s">
-        <v>50</v>
       </c>
       <c r="O6">
         <v>7</v>
       </c>
       <c r="P6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="R6" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18">
       <c r="A7" t="s">
         <v>18</v>
       </c>
       <c r="C7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D7">
         <v>0</v>
@@ -1318,28 +1342,28 @@
         <v>4</v>
       </c>
       <c r="K7" t="s">
+        <v>53</v>
+      </c>
+      <c r="L7" t="s">
         <v>54</v>
       </c>
-      <c r="L7" t="s">
+      <c r="M7" t="s">
         <v>55</v>
       </c>
-      <c r="M7" t="s">
-        <v>56</v>
-      </c>
       <c r="N7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="O7">
         <v>26</v>
       </c>
       <c r="P7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="R7" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18">
       <c r="A8" t="s">
         <v>18</v>
       </c>
@@ -1356,7 +1380,7 @@
         <v>0</v>
       </c>
       <c r="G8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H8" t="s">
         <v>26</v>
@@ -1368,28 +1392,28 @@
         <v>4</v>
       </c>
       <c r="K8" t="s">
+        <v>56</v>
+      </c>
+      <c r="L8" t="s">
         <v>57</v>
       </c>
-      <c r="L8" t="s">
+      <c r="M8" t="s">
         <v>58</v>
       </c>
-      <c r="M8" t="s">
+      <c r="N8" t="s">
         <v>59</v>
       </c>
-      <c r="N8" t="s">
-        <v>60</v>
-      </c>
       <c r="O8">
         <v>26</v>
       </c>
       <c r="P8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="R8" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18">
       <c r="A9" t="s">
         <v>18</v>
       </c>
@@ -1409,37 +1433,37 @@
         <v>0</v>
       </c>
       <c r="H9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="I9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J9" t="s">
         <v>4</v>
       </c>
       <c r="K9" t="s">
+        <v>65</v>
+      </c>
+      <c r="L9" t="s">
+        <v>54</v>
+      </c>
+      <c r="M9" t="s">
+        <v>29</v>
+      </c>
+      <c r="N9" t="s">
         <v>66</v>
       </c>
-      <c r="L9" t="s">
-        <v>55</v>
-      </c>
-      <c r="M9" t="s">
-        <v>30</v>
-      </c>
-      <c r="N9" t="s">
-        <v>67</v>
-      </c>
       <c r="O9">
         <v>26</v>
       </c>
       <c r="P9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="R9" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18">
       <c r="A10" t="s">
         <v>18</v>
       </c>
@@ -1453,7 +1477,7 @@
         <v>0</v>
       </c>
       <c r="F10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G10">
         <v>0</v>
@@ -1468,28 +1492,28 @@
         <v>4</v>
       </c>
       <c r="K10" t="s">
+        <v>61</v>
+      </c>
+      <c r="L10" t="s">
+        <v>72</v>
+      </c>
+      <c r="M10" t="s">
         <v>62</v>
       </c>
-      <c r="L10" t="s">
-        <v>73</v>
-      </c>
-      <c r="M10" t="s">
+      <c r="N10" t="s">
         <v>63</v>
       </c>
-      <c r="N10" t="s">
-        <v>64</v>
-      </c>
       <c r="O10">
         <v>26</v>
       </c>
       <c r="P10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="R10" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18">
       <c r="A11" t="s">
         <v>18</v>
       </c>
@@ -1518,36 +1542,36 @@
         <v>4</v>
       </c>
       <c r="K11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="L11" t="s">
+        <v>76</v>
+      </c>
+      <c r="M11" t="s">
         <v>77</v>
       </c>
-      <c r="M11" t="s">
-        <v>78</v>
-      </c>
       <c r="N11" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="O11">
         <v>26</v>
       </c>
       <c r="P11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="R11" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18">
       <c r="A12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C12">
         <v>0</v>
       </c>
       <c r="F12" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G12">
         <v>0</v>
@@ -1562,30 +1586,30 @@
         <v>4</v>
       </c>
       <c r="K12" t="s">
+        <v>73</v>
+      </c>
+      <c r="L12" t="s">
         <v>74</v>
       </c>
-      <c r="L12" t="s">
+      <c r="M12" t="s">
         <v>75</v>
       </c>
-      <c r="M12" t="s">
-        <v>76</v>
-      </c>
       <c r="N12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="O12">
         <v>18</v>
       </c>
       <c r="P12" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="R12" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18">
       <c r="A13" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C13" t="s">
         <v>20</v>
@@ -1612,28 +1636,28 @@
         <v>4</v>
       </c>
       <c r="K13" t="s">
+        <v>80</v>
+      </c>
+      <c r="L13" t="s">
         <v>81</v>
       </c>
-      <c r="L13" t="s">
+      <c r="M13" t="s">
         <v>82</v>
       </c>
-      <c r="M13" t="s">
+      <c r="N13" t="s">
         <v>83</v>
-      </c>
-      <c r="N13" t="s">
-        <v>84</v>
       </c>
       <c r="O13">
         <v>18</v>
       </c>
       <c r="P13" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="R13" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18">
       <c r="A14" t="s">
         <v>18</v>
       </c>
@@ -1659,89 +1683,89 @@
         <v>4</v>
       </c>
       <c r="K14" t="s">
+        <v>84</v>
+      </c>
+      <c r="L14" t="s">
         <v>85</v>
       </c>
-      <c r="L14" t="s">
+      <c r="M14" t="s">
         <v>86</v>
       </c>
-      <c r="M14" t="s">
+      <c r="N14" t="s">
         <v>87</v>
       </c>
-      <c r="N14" t="s">
-        <v>88</v>
-      </c>
       <c r="O14">
         <v>26</v>
       </c>
       <c r="P14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="R14" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18">
       <c r="A15" t="s">
         <v>18</v>
       </c>
       <c r="J15" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="K15">
         <v>1</v>
       </c>
       <c r="L15" t="s">
+        <v>95</v>
+      </c>
+      <c r="M15" t="s">
         <v>96</v>
       </c>
-      <c r="M15" t="s">
+      <c r="N15" t="s">
         <v>97</v>
       </c>
-      <c r="N15" t="s">
-        <v>98</v>
-      </c>
       <c r="O15">
         <v>26</v>
       </c>
       <c r="P15" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="R15" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18">
       <c r="A16" t="s">
         <v>18</v>
       </c>
       <c r="J16" t="s">
+        <v>105</v>
+      </c>
+      <c r="K16" t="s">
         <v>106</v>
       </c>
-      <c r="K16" t="s">
+      <c r="L16" t="s">
         <v>107</v>
       </c>
-      <c r="L16" t="s">
+      <c r="M16" t="s">
         <v>108</v>
       </c>
-      <c r="M16" t="s">
+      <c r="N16" t="s">
         <v>109</v>
       </c>
-      <c r="N16" t="s">
-        <v>110</v>
-      </c>
       <c r="O16">
         <v>26</v>
       </c>
       <c r="P16" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="Q16">
         <v>14002</v>
       </c>
       <c r="R16" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.2">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15">
       <c r="A38" s="1" t="s">
         <v>16</v>
       </c>
@@ -1759,12 +1783,12 @@
       <c r="M38" s="1"/>
       <c r="N38" s="1"/>
     </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:15">
       <c r="A39" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>17</v>
@@ -1779,7 +1803,7 @@
         <v>14</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H39" s="1" t="s">
         <v>15</v>
@@ -1800,18 +1824,18 @@
         <v>25</v>
       </c>
       <c r="N39" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="O39" s="1" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.2">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15">
       <c r="A40" t="s">
         <v>18</v>
       </c>
       <c r="C40" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D40">
         <v>0</v>
@@ -1829,33 +1853,33 @@
         <v>4</v>
       </c>
       <c r="I40" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="J40" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="J40" s="3" t="s">
+      <c r="K40" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="K40" s="3" t="s">
+      <c r="L40" t="s">
         <v>137</v>
       </c>
-      <c r="L40" t="s">
-        <v>138</v>
-      </c>
       <c r="M40">
         <v>26</v>
       </c>
       <c r="N40" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="O40" s="3">
         <v>72.700999999999993</v>
       </c>
     </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:15">
       <c r="A41" t="s">
         <v>18</v>
       </c>
       <c r="D41" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E41" t="s">
         <v>20</v>
@@ -1867,41 +1891,41 @@
         <v>4</v>
       </c>
       <c r="I41" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="J41" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="J41" s="3" t="s">
+      <c r="K41" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="K41" s="3" t="s">
+      <c r="L41" t="s">
         <v>141</v>
       </c>
-      <c r="L41" t="s">
-        <v>142</v>
-      </c>
       <c r="M41">
         <v>26</v>
       </c>
       <c r="N41" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="O41" s="3">
         <v>5.0039999999999996</v>
       </c>
     </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:15">
       <c r="A42" t="s">
+        <v>67</v>
+      </c>
+      <c r="L42" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15">
+      <c r="A43" t="s">
         <v>68</v>
       </c>
-      <c r="L42" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
-        <v>69</v>
-      </c>
       <c r="C43" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D43">
         <v>0</v>
@@ -1919,30 +1943,30 @@
         <v>4</v>
       </c>
       <c r="I43" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="J43" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="J43" s="3" t="s">
+      <c r="K43" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="K43" s="3" t="s">
+      <c r="L43" t="s">
         <v>133</v>
-      </c>
-      <c r="L43" t="s">
-        <v>134</v>
       </c>
       <c r="M43">
         <v>20</v>
       </c>
       <c r="N43" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="O43" s="3">
         <v>262.065</v>
       </c>
     </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:15">
       <c r="A44" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D44" t="s">
         <v>20</v>
@@ -1951,105 +1975,105 @@
         <v>19</v>
       </c>
       <c r="F44" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H44" t="s">
         <v>4</v>
       </c>
       <c r="I44" t="s">
+        <v>89</v>
+      </c>
+      <c r="J44" t="s">
+        <v>78</v>
+      </c>
+      <c r="K44" t="s">
         <v>90</v>
       </c>
-      <c r="J44" t="s">
-        <v>79</v>
-      </c>
-      <c r="K44" t="s">
+      <c r="L44" t="s">
         <v>91</v>
-      </c>
-      <c r="L44" t="s">
-        <v>92</v>
       </c>
       <c r="M44">
         <v>20</v>
       </c>
       <c r="N44" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="O44">
         <v>1162680</v>
       </c>
     </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:15">
       <c r="A45" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="O45" s="4" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.2">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15">
       <c r="A46" t="s">
         <v>18</v>
       </c>
       <c r="H46" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="I46">
         <v>1</v>
       </c>
       <c r="J46" t="s">
+        <v>111</v>
+      </c>
+      <c r="K46" t="s">
         <v>112</v>
       </c>
-      <c r="K46" t="s">
+      <c r="L46" t="s">
         <v>113</v>
       </c>
-      <c r="L46" t="s">
-        <v>114</v>
-      </c>
       <c r="M46">
         <v>26</v>
       </c>
       <c r="N46" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="O46">
         <v>9931</v>
       </c>
     </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:15">
       <c r="A47" t="s">
         <v>18</v>
       </c>
       <c r="H47" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="I47">
         <v>1</v>
       </c>
       <c r="J47" t="s">
+        <v>111</v>
+      </c>
+      <c r="K47" t="s">
         <v>112</v>
       </c>
-      <c r="K47" t="s">
-        <v>113</v>
-      </c>
       <c r="L47" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="M47">
         <v>26</v>
       </c>
       <c r="N47" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="O47">
         <v>9856</v>
       </c>
     </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:15">
       <c r="A48" t="s">
         <v>18</v>
       </c>
       <c r="D48" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E48" t="s">
         <v>19</v>
@@ -2061,33 +2085,33 @@
         <v>4</v>
       </c>
       <c r="I48" t="s">
+        <v>119</v>
+      </c>
+      <c r="J48" t="s">
         <v>120</v>
       </c>
-      <c r="J48" t="s">
+      <c r="K48" t="s">
         <v>121</v>
       </c>
-      <c r="K48" t="s">
+      <c r="L48" t="s">
         <v>122</v>
-      </c>
-      <c r="L48" t="s">
-        <v>123</v>
       </c>
       <c r="M48">
         <v>20</v>
       </c>
       <c r="N48" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="O48" s="3">
         <v>1.6639999999999999</v>
       </c>
     </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:15">
       <c r="A49" t="s">
         <v>18</v>
       </c>
       <c r="B49" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E49" t="s">
         <v>19</v>
@@ -2099,205 +2123,259 @@
         <v>4</v>
       </c>
       <c r="I49" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="J49" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="J49" s="3" t="s">
+      <c r="K49" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="K49" s="3" t="s">
+      <c r="L49" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="L49" s="3" t="s">
+      <c r="N49" s="3" t="s">
         <v>129</v>
-      </c>
-      <c r="N49" s="3" t="s">
-        <v>130</v>
       </c>
       <c r="O49" s="3">
         <v>37.241999999999997</v>
       </c>
     </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:15">
       <c r="A54" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C54" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B54" s="1"/>
-      <c r="C54" s="1"/>
-      <c r="D54" s="1"/>
-      <c r="E54" s="1"/>
-      <c r="F54" s="1"/>
-      <c r="G54" s="1"/>
-      <c r="H54" s="1"/>
-      <c r="I54" s="1"/>
-      <c r="J54" s="1"/>
-      <c r="K54" s="1"/>
-      <c r="L54" s="1"/>
-    </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A55" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B55" s="1"/>
-      <c r="C55" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D55" s="1" t="s">
+      <c r="D54" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E54" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F54" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G54" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H54" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I54" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J54" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="K54" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="L54" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="55" spans="1:15">
+      <c r="A55" t="s">
+        <v>18</v>
+      </c>
+      <c r="B55" t="s">
         <v>28</v>
       </c>
-      <c r="E55" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F55" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G55" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="H55" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="I55" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="J55" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="K55" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="L55" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="M55" s="1" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="C55">
+        <v>0</v>
+      </c>
+      <c r="D55" t="s">
+        <v>20</v>
+      </c>
+      <c r="E55" t="s">
+        <v>4</v>
+      </c>
+      <c r="F55" t="s">
+        <v>29</v>
+      </c>
+      <c r="G55" t="s">
+        <v>30</v>
+      </c>
+      <c r="H55" t="s">
+        <v>31</v>
+      </c>
+      <c r="I55" t="s">
+        <v>32</v>
+      </c>
+      <c r="J55">
+        <v>26</v>
+      </c>
+      <c r="K55" t="s">
+        <v>104</v>
+      </c>
+      <c r="L55">
+        <v>8841</v>
+      </c>
+      <c r="M55" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="56" spans="1:15">
       <c r="A56" t="s">
         <v>18</v>
       </c>
+      <c r="B56" t="s">
+        <v>28</v>
+      </c>
       <c r="C56" t="s">
-        <v>29</v>
-      </c>
-      <c r="D56">
-        <v>0</v>
+        <v>28</v>
+      </c>
+      <c r="D56" t="s">
+        <v>20</v>
       </c>
       <c r="E56" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="F56" t="s">
-        <v>4</v>
+        <v>100</v>
       </c>
       <c r="G56" t="s">
-        <v>30</v>
+        <v>101</v>
       </c>
       <c r="H56" t="s">
-        <v>31</v>
+        <v>102</v>
       </c>
       <c r="I56" t="s">
-        <v>32</v>
-      </c>
-      <c r="J56" t="s">
-        <v>33</v>
-      </c>
-      <c r="K56">
-        <v>26</v>
-      </c>
-      <c r="L56" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.2">
+        <v>103</v>
+      </c>
+      <c r="J56">
+        <v>26</v>
+      </c>
+      <c r="K56" t="s">
+        <v>104</v>
+      </c>
+      <c r="L56" s="2">
+        <v>5590</v>
+      </c>
+      <c r="M56" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="57" spans="1:15">
       <c r="A57" t="s">
         <v>18</v>
       </c>
-      <c r="C57" t="s">
-        <v>29</v>
+      <c r="B57" t="s">
+        <v>99</v>
+      </c>
+      <c r="C57">
+        <v>0</v>
       </c>
       <c r="D57" t="s">
-        <v>29</v>
+        <v>60</v>
       </c>
       <c r="E57" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="F57" t="s">
-        <v>4</v>
+        <v>114</v>
       </c>
       <c r="G57" t="s">
-        <v>101</v>
+        <v>115</v>
       </c>
       <c r="H57" t="s">
-        <v>102</v>
+        <v>116</v>
       </c>
       <c r="I57" t="s">
-        <v>103</v>
-      </c>
-      <c r="J57" t="s">
+        <v>117</v>
+      </c>
+      <c r="J57">
+        <v>26</v>
+      </c>
+      <c r="K57" t="s">
         <v>104</v>
       </c>
-      <c r="K57">
-        <v>26</v>
-      </c>
-      <c r="L57" t="s">
-        <v>105</v>
-      </c>
-      <c r="M57" s="2">
-        <v>5590</v>
-      </c>
-    </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="L57" s="2">
+        <v>6912</v>
+      </c>
+      <c r="M57" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="58" spans="1:15">
       <c r="A58" t="s">
         <v>18</v>
       </c>
+      <c r="B58" t="s">
+        <v>142</v>
+      </c>
       <c r="C58" t="s">
-        <v>100</v>
-      </c>
-      <c r="D58">
-        <v>0</v>
+        <v>143</v>
+      </c>
+      <c r="D58" t="s">
+        <v>144</v>
       </c>
       <c r="E58" t="s">
-        <v>61</v>
+        <v>4</v>
       </c>
       <c r="F58" t="s">
-        <v>4</v>
+        <v>145</v>
       </c>
       <c r="G58" t="s">
-        <v>115</v>
+        <v>146</v>
       </c>
       <c r="H58" t="s">
-        <v>116</v>
+        <v>147</v>
       </c>
       <c r="I58" t="s">
-        <v>117</v>
-      </c>
-      <c r="J58" t="s">
-        <v>118</v>
-      </c>
-      <c r="K58">
-        <v>26</v>
-      </c>
-      <c r="L58" t="s">
-        <v>105</v>
-      </c>
-      <c r="M58" s="2">
-        <v>6912</v>
-      </c>
-    </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.2">
+        <v>148</v>
+      </c>
+      <c r="J58">
+        <v>26</v>
+      </c>
+      <c r="K58" t="s">
+        <v>104</v>
+      </c>
+      <c r="L58" s="2">
+        <v>3286</v>
+      </c>
+    </row>
+    <row r="59" spans="1:15">
       <c r="A59" t="s">
         <v>18</v>
       </c>
-      <c r="C59">
-        <v>0</v>
+      <c r="B59" t="s">
+        <v>142</v>
+      </c>
+      <c r="C59" t="s">
+        <v>99</v>
+      </c>
+      <c r="D59" t="s">
+        <v>60</v>
+      </c>
+      <c r="E59" t="s">
+        <v>4</v>
       </c>
       <c r="F59" t="s">
-        <v>4</v>
-      </c>
-      <c r="K59">
-        <v>26</v>
-      </c>
-      <c r="L59" t="s">
-        <v>105</v>
+        <v>149</v>
+      </c>
+      <c r="G59" t="s">
+        <v>150</v>
+      </c>
+      <c r="H59" t="s">
+        <v>151</v>
+      </c>
+      <c r="I59" t="s">
+        <v>152</v>
+      </c>
+      <c r="J59">
+        <v>26</v>
+      </c>
+      <c r="K59" t="s">
+        <v>104</v>
+      </c>
+      <c r="L59" s="2">
+        <v>3367</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add final ir results of transfer api
</commit_message>
<xml_diff>
--- a/IdentityResolutionExperimentation/identity_resolution_results.xlsx
+++ b/IdentityResolutionExperimentation/identity_resolution_results.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22130"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26621"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\linar\OneDrive\Документы\GitHub\WDI_2019\IdentityResolutionExperimentation\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CEDCEE1-3FFC-4845-92F4-B1E1318FB2F6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1860" yWindow="1240" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Blatt2" sheetId="2" r:id="rId1"/>
@@ -25,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="171">
   <si>
     <t>Blocker</t>
   </si>
@@ -462,15 +456,6 @@
     <t>0.15</t>
   </si>
   <si>
-    <t>0.9519</t>
-  </si>
-  <si>
-    <t>0.7984</t>
-  </si>
-  <si>
-    <t>0.8684</t>
-  </si>
-  <si>
     <t>2 Minutes 44 Seconds</t>
   </si>
   <si>
@@ -483,9 +468,6 @@
     <t>0.8634</t>
   </si>
   <si>
-    <t>2 Minutes 25 Seconds</t>
-  </si>
-  <si>
     <t>0.81</t>
   </si>
   <si>
@@ -541,13 +523,22 @@
   </si>
   <si>
     <t>0.78</t>
+  </si>
+  <si>
+    <t>0.79</t>
+  </si>
+  <si>
+    <t>0.9703</t>
+  </si>
+  <si>
+    <t>0.8711</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -690,75 +681,75 @@
     </xf>
   </cellXfs>
   <cellStyles count="69">
-    <cellStyle name="Гиперссылка" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Гиперссылка" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Гиперссылка" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="Гиперссылка" xfId="7" builtinId="8" hidden="1"/>
-    <cellStyle name="Гиперссылка" xfId="9" builtinId="8" hidden="1"/>
-    <cellStyle name="Гиперссылка" xfId="11" builtinId="8" hidden="1"/>
-    <cellStyle name="Гиперссылка" xfId="13" builtinId="8" hidden="1"/>
-    <cellStyle name="Гиперссылка" xfId="15" builtinId="8" hidden="1"/>
-    <cellStyle name="Гиперссылка" xfId="17" builtinId="8" hidden="1"/>
-    <cellStyle name="Гиперссылка" xfId="19" builtinId="8" hidden="1"/>
-    <cellStyle name="Гиперссылка" xfId="21" builtinId="8" hidden="1"/>
-    <cellStyle name="Гиперссылка" xfId="23" builtinId="8" hidden="1"/>
-    <cellStyle name="Гиперссылка" xfId="25" builtinId="8" hidden="1"/>
-    <cellStyle name="Гиперссылка" xfId="27" builtinId="8" hidden="1"/>
-    <cellStyle name="Гиперссылка" xfId="29" builtinId="8" hidden="1"/>
-    <cellStyle name="Гиперссылка" xfId="31" builtinId="8" hidden="1"/>
-    <cellStyle name="Гиперссылка" xfId="33" builtinId="8" hidden="1"/>
-    <cellStyle name="Гиперссылка" xfId="35" builtinId="8" hidden="1"/>
-    <cellStyle name="Гиперссылка" xfId="37" builtinId="8" hidden="1"/>
-    <cellStyle name="Гиперссылка" xfId="39" builtinId="8" hidden="1"/>
-    <cellStyle name="Гиперссылка" xfId="41" builtinId="8" hidden="1"/>
-    <cellStyle name="Гиперссылка" xfId="43" builtinId="8" hidden="1"/>
-    <cellStyle name="Гиперссылка" xfId="45" builtinId="8" hidden="1"/>
-    <cellStyle name="Гиперссылка" xfId="47" builtinId="8" hidden="1"/>
-    <cellStyle name="Гиперссылка" xfId="49" builtinId="8" hidden="1"/>
-    <cellStyle name="Гиперссылка" xfId="51" builtinId="8" hidden="1"/>
-    <cellStyle name="Гиперссылка" xfId="53" builtinId="8" hidden="1"/>
-    <cellStyle name="Гиперссылка" xfId="55" builtinId="8" hidden="1"/>
-    <cellStyle name="Гиперссылка" xfId="57" builtinId="8" hidden="1"/>
-    <cellStyle name="Гиперссылка" xfId="59" builtinId="8" hidden="1"/>
-    <cellStyle name="Гиперссылка" xfId="61" builtinId="8" hidden="1"/>
-    <cellStyle name="Гиперссылка" xfId="63" builtinId="8" hidden="1"/>
-    <cellStyle name="Гиперссылка" xfId="65" builtinId="8" hidden="1"/>
-    <cellStyle name="Гиперссылка" xfId="67" builtinId="8" hidden="1"/>
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
-    <cellStyle name="Открывавшаяся гиперссылка" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Открывавшаяся гиперссылка" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Открывавшаяся гиперссылка" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Открывавшаяся гиперссылка" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Открывавшаяся гиперссылка" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Открывавшаяся гиперссылка" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="Открывавшаяся гиперссылка" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="Открывавшаяся гиперссылка" xfId="16" builtinId="9" hidden="1"/>
-    <cellStyle name="Открывавшаяся гиперссылка" xfId="18" builtinId="9" hidden="1"/>
-    <cellStyle name="Открывавшаяся гиперссылка" xfId="20" builtinId="9" hidden="1"/>
-    <cellStyle name="Открывавшаяся гиперссылка" xfId="22" builtinId="9" hidden="1"/>
-    <cellStyle name="Открывавшаяся гиперссылка" xfId="24" builtinId="9" hidden="1"/>
-    <cellStyle name="Открывавшаяся гиперссылка" xfId="26" builtinId="9" hidden="1"/>
-    <cellStyle name="Открывавшаяся гиперссылка" xfId="28" builtinId="9" hidden="1"/>
-    <cellStyle name="Открывавшаяся гиперссылка" xfId="30" builtinId="9" hidden="1"/>
-    <cellStyle name="Открывавшаяся гиперссылка" xfId="32" builtinId="9" hidden="1"/>
-    <cellStyle name="Открывавшаяся гиперссылка" xfId="34" builtinId="9" hidden="1"/>
-    <cellStyle name="Открывавшаяся гиперссылка" xfId="36" builtinId="9" hidden="1"/>
-    <cellStyle name="Открывавшаяся гиперссылка" xfId="38" builtinId="9" hidden="1"/>
-    <cellStyle name="Открывавшаяся гиперссылка" xfId="40" builtinId="9" hidden="1"/>
-    <cellStyle name="Открывавшаяся гиперссылка" xfId="42" builtinId="9" hidden="1"/>
-    <cellStyle name="Открывавшаяся гиперссылка" xfId="44" builtinId="9" hidden="1"/>
-    <cellStyle name="Открывавшаяся гиперссылка" xfId="46" builtinId="9" hidden="1"/>
-    <cellStyle name="Открывавшаяся гиперссылка" xfId="48" builtinId="9" hidden="1"/>
-    <cellStyle name="Открывавшаяся гиперссылка" xfId="50" builtinId="9" hidden="1"/>
-    <cellStyle name="Открывавшаяся гиперссылка" xfId="52" builtinId="9" hidden="1"/>
-    <cellStyle name="Открывавшаяся гиперссылка" xfId="54" builtinId="9" hidden="1"/>
-    <cellStyle name="Открывавшаяся гиперссылка" xfId="56" builtinId="9" hidden="1"/>
-    <cellStyle name="Открывавшаяся гиперссылка" xfId="58" builtinId="9" hidden="1"/>
-    <cellStyle name="Открывавшаяся гиперссылка" xfId="60" builtinId="9" hidden="1"/>
-    <cellStyle name="Открывавшаяся гиперссылка" xfId="62" builtinId="9" hidden="1"/>
-    <cellStyle name="Открывавшаяся гиперссылка" xfId="64" builtinId="9" hidden="1"/>
-    <cellStyle name="Открывавшаяся гиперссылка" xfId="66" builtinId="9" hidden="1"/>
-    <cellStyle name="Открывавшаяся гиперссылка" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Link" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -1094,14 +1085,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R59"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" topLeftCell="C16" zoomScale="75" workbookViewId="0">
+      <selection activeCell="L58" sqref="L58"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="44.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="44.33203125" customWidth="1"/>
@@ -1223,7 +1214,7 @@
         <v>6</v>
       </c>
       <c r="O3" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="P3">
         <v>18246</v>
@@ -1338,7 +1329,7 @@
         <v>28</v>
       </c>
       <c r="R5" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
     </row>
     <row r="6" spans="1:18">
@@ -1444,7 +1435,7 @@
         <v>28</v>
       </c>
       <c r="R7" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
     </row>
     <row r="8" spans="1:18">
@@ -1529,16 +1520,16 @@
         <v>4</v>
       </c>
       <c r="J9" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="K9" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="L9" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="M9" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="N9">
         <v>26</v>
@@ -1550,10 +1541,10 @@
         <v>4238</v>
       </c>
       <c r="Q9" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="R9" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
     </row>
     <row r="10" spans="1:18">
@@ -1659,7 +1650,7 @@
         <v>28</v>
       </c>
       <c r="R11" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
     </row>
     <row r="12" spans="1:18">
@@ -1715,7 +1706,7 @@
         <v>28</v>
       </c>
       <c r="R12" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
     </row>
     <row r="13" spans="1:18">
@@ -1747,16 +1738,16 @@
         <v>4</v>
       </c>
       <c r="J13" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="K13" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="L13" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="M13" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="N13">
         <v>26</v>
@@ -1768,7 +1759,7 @@
         <v>4546</v>
       </c>
       <c r="Q13" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
     </row>
     <row r="14" spans="1:18">
@@ -1803,13 +1794,13 @@
         <v>130</v>
       </c>
       <c r="K14" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="L14" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="M14" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="N14">
         <v>26</v>
@@ -1821,7 +1812,7 @@
         <v>3944</v>
       </c>
       <c r="Q14" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
     </row>
     <row r="15" spans="1:18">
@@ -2091,7 +2082,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="40" spans="1:15">
+    <row r="40" spans="1:15" ht="16">
       <c r="A40" t="s">
         <v>18</v>
       </c>
@@ -2135,7 +2126,7 @@
         <v>72.700999999999993</v>
       </c>
     </row>
-    <row r="41" spans="1:15">
+    <row r="41" spans="1:15" ht="16">
       <c r="A41" t="s">
         <v>18</v>
       </c>
@@ -2181,7 +2172,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="43" spans="1:15">
+    <row r="43" spans="1:15" ht="16">
       <c r="A43" t="s">
         <v>68</v>
       </c>
@@ -2329,7 +2320,7 @@
         <v>9856</v>
       </c>
     </row>
-    <row r="48" spans="1:15">
+    <row r="48" spans="1:15" ht="16">
       <c r="A48" t="s">
         <v>18</v>
       </c>
@@ -2367,7 +2358,7 @@
         <v>1.6639999999999999</v>
       </c>
     </row>
-    <row r="49" spans="1:15">
+    <row r="49" spans="1:15" ht="16">
       <c r="A49" t="s">
         <v>18</v>
       </c>
@@ -2438,6 +2429,9 @@
       </c>
       <c r="L54" s="1" t="s">
         <v>88</v>
+      </c>
+      <c r="M54" s="1" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="55" spans="1:15">
@@ -2580,16 +2574,16 @@
         <v>4</v>
       </c>
       <c r="F58" t="s">
+        <v>169</v>
+      </c>
+      <c r="G58" t="s">
+        <v>147</v>
+      </c>
+      <c r="H58" t="s">
+        <v>170</v>
+      </c>
+      <c r="I58" t="s">
         <v>145</v>
-      </c>
-      <c r="G58" t="s">
-        <v>146</v>
-      </c>
-      <c r="H58" t="s">
-        <v>147</v>
-      </c>
-      <c r="I58" t="s">
-        <v>148</v>
       </c>
       <c r="J58">
         <v>26</v>
@@ -2598,7 +2592,10 @@
         <v>104</v>
       </c>
       <c r="L58" s="2">
-        <v>3286</v>
+        <v>3026</v>
+      </c>
+      <c r="M58" t="s">
+        <v>168</v>
       </c>
     </row>
     <row r="59" spans="1:15">
@@ -2618,16 +2615,16 @@
         <v>4</v>
       </c>
       <c r="F59" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="G59" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="H59" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="I59" t="s">
-        <v>152</v>
+        <v>163</v>
       </c>
       <c r="J59">
         <v>26</v>
@@ -2636,7 +2633,10 @@
         <v>104</v>
       </c>
       <c r="L59" s="2">
-        <v>3367</v>
+        <v>3070</v>
+      </c>
+      <c r="M59" t="s">
+        <v>168</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add most recent ir results
</commit_message>
<xml_diff>
--- a/IdentityResolutionExperimentation/identity_resolution_results.xlsx
+++ b/IdentityResolutionExperimentation/identity_resolution_results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26621"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="1240" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Blatt2" sheetId="2" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="461" uniqueCount="197">
   <si>
     <t>Blocker</t>
   </si>
@@ -141,9 +141,6 @@
     <t xml:space="preserve"> 0 Minutes 20 Seconds</t>
   </si>
   <si>
-    <t>Height: Percentage Differences</t>
-  </si>
-  <si>
     <t>4 Minutes 34 Seconds</t>
   </si>
   <si>
@@ -231,9 +228,6 @@
     <t>0.89</t>
   </si>
   <si>
-    <t>0.934</t>
-  </si>
-  <si>
     <t>0.948</t>
   </si>
   <si>
@@ -354,15 +348,9 @@
     <t>ML: SimpleLogistic</t>
   </si>
   <si>
-    <t>0.795</t>
-  </si>
-  <si>
     <t>0.8864</t>
   </si>
   <si>
-    <t>10 Minutes 2 Seconds</t>
-  </si>
-  <si>
     <t>0.8702</t>
   </si>
   <si>
@@ -375,42 +363,6 @@
     <t>2 Minutes 47 Seconds</t>
   </si>
   <si>
-    <t>13 Minutes 2 Seconds</t>
-  </si>
-  <si>
-    <t>1.00</t>
-  </si>
-  <si>
-    <t>0.1885</t>
-  </si>
-  <si>
-    <t>0.3127</t>
-  </si>
-  <si>
-    <t>2 Minutes 39 seconds</t>
-  </si>
-  <si>
-    <t xml:space="preserve">≈526 </t>
-  </si>
-  <si>
-    <t>Name: Comparator</t>
-  </si>
-  <si>
-    <t>0.9904</t>
-  </si>
-  <si>
-    <t>0.5393</t>
-  </si>
-  <si>
-    <t>0.6983</t>
-  </si>
-  <si>
-    <t>3 Minutes 40 Seconds</t>
-  </si>
-  <si>
-    <t> 0.934</t>
-  </si>
-  <si>
     <t>0.9688</t>
   </si>
   <si>
@@ -423,30 +375,6 @@
     <t>2 Minutes 34 Seconds</t>
   </si>
   <si>
-    <t>0.9854</t>
-  </si>
-  <si>
-    <t> 0.7068</t>
-  </si>
-  <si>
-    <t>0.8232</t>
-  </si>
-  <si>
-    <t>2 Minutes 21 Seconds</t>
-  </si>
-  <si>
-    <t>0.9889</t>
-  </si>
-  <si>
-    <t>0.4660</t>
-  </si>
-  <si>
-    <t>0.6335</t>
-  </si>
-  <si>
-    <t>2 Minutes 22 Seconds</t>
-  </si>
-  <si>
     <t>Extra Information: sim=1 if Levenshtein =1 and and date_sim != 0</t>
   </si>
   <si>
@@ -532,6 +460,156 @@
   </si>
   <si>
     <t>0.8711</t>
+  </si>
+  <si>
+    <t>0.7959</t>
+  </si>
+  <si>
+    <t>0.6</t>
+  </si>
+  <si>
+    <t>0.4</t>
+  </si>
+  <si>
+    <t>0.82</t>
+  </si>
+  <si>
+    <t>Extra Information: sim=1 if Levenshtein =1 and and date_sim != 1</t>
+  </si>
+  <si>
+    <t>2 Minutes 51 Seconds</t>
+  </si>
+  <si>
+    <t>0.83</t>
+  </si>
+  <si>
+    <t>reduces wrong overlapping correspondences</t>
+  </si>
+  <si>
+    <t>0.84</t>
+  </si>
+  <si>
+    <t>Extra Information: sim=1 if Levenshtein =1 and and date_sim != 2</t>
+  </si>
+  <si>
+    <t>3 Mintues 5 Seconds</t>
+  </si>
+  <si>
+    <t>0.86</t>
+  </si>
+  <si>
+    <t>Extra Information: sim=1 if Levenshtein =1 and and date_sim != 3</t>
+  </si>
+  <si>
+    <t>Extra Information: sim=1 if Levenshtein =1 and and date_sim != 4</t>
+  </si>
+  <si>
+    <t>2 Minutes 52 Seconds</t>
+  </si>
+  <si>
+    <t>2 Mintues 51 Seconds</t>
+  </si>
+  <si>
+    <t>0.5645</t>
+  </si>
+  <si>
+    <t>0.7216</t>
+  </si>
+  <si>
+    <t>&gt; limit reached!</t>
+  </si>
+  <si>
+    <t>3 Minutes 15 Seconds</t>
+  </si>
+  <si>
+    <t>0.9675</t>
+  </si>
+  <si>
+    <t>0.7720</t>
+  </si>
+  <si>
+    <t>3 Minutes 23 sEconds</t>
+  </si>
+  <si>
+    <t>0.9885</t>
+  </si>
+  <si>
+    <t>0.4526</t>
+  </si>
+  <si>
+    <t>0.6209</t>
+  </si>
+  <si>
+    <t>5 Minutes 26 Seconds</t>
+  </si>
+  <si>
+    <t>False Fusion</t>
+  </si>
+  <si>
+    <t>Very bad</t>
+  </si>
+  <si>
+    <t>17 False Fusion</t>
+  </si>
+  <si>
+    <t>0.8588</t>
+  </si>
+  <si>
+    <t>0.3947</t>
+  </si>
+  <si>
+    <t>0.566</t>
+  </si>
+  <si>
+    <t>2 Minutes 15 Seconds</t>
+  </si>
+  <si>
+    <t>17 wrong</t>
+  </si>
+  <si>
+    <t>0.9787</t>
+  </si>
+  <si>
+    <t>0.7150</t>
+  </si>
+  <si>
+    <t>0.8263</t>
+  </si>
+  <si>
+    <t>3 Minutes 6 Seconds</t>
+  </si>
+  <si>
+    <t>13 False</t>
+  </si>
+  <si>
+    <t>140 wrong</t>
+  </si>
+  <si>
+    <t>0.35</t>
+  </si>
+  <si>
+    <t>3 Minutes 7 Secondes</t>
+  </si>
+  <si>
+    <t>160 wronf</t>
+  </si>
+  <si>
+    <t>0.9850</t>
+  </si>
+  <si>
+    <t>0.6895</t>
+  </si>
+  <si>
+    <t>0.8111</t>
+  </si>
+  <si>
+    <t>2 Minutes 19 Seconds</t>
+  </si>
+  <si>
+    <t>108 wrong</t>
+  </si>
+  <si>
+    <t>0.985</t>
   </si>
 </sst>
 </file>
@@ -583,12 +661,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -600,7 +684,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="69">
+  <cellStyleXfs count="111">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -670,8 +754,50 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -679,8 +805,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="69">
+  <cellStyles count="111">
     <cellStyle name="Besuchter Link" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="6" builtinId="9" hidden="1"/>
@@ -715,6 +843,27 @@
     <cellStyle name="Besuchter Link" xfId="64" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="66" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="98" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="100" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="104" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="106" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="108" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="110" builtinId="9" hidden="1"/>
     <cellStyle name="Link" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="5" builtinId="8" hidden="1"/>
@@ -749,6 +898,27 @@
     <cellStyle name="Link" xfId="63" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="65" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="93" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="95" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="97" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="99" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="101" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="103" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="105" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="107" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="109" builtinId="8" hidden="1"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1086,10 +1256,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R59"/>
+  <dimension ref="A1:R70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C16" zoomScale="75" workbookViewId="0">
-      <selection activeCell="L58" sqref="L58"/>
+    <sheetView tabSelected="1" topLeftCell="E27" zoomScale="75" workbookViewId="0">
+      <selection activeCell="O61" sqref="O61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1163,10 +1333,10 @@
         <v>36</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="Q2" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="R2" s="1"/>
     </row>
@@ -1214,7 +1384,7 @@
         <v>6</v>
       </c>
       <c r="O3" t="s">
-        <v>149</v>
+        <v>125</v>
       </c>
       <c r="P3">
         <v>18246</v>
@@ -1305,16 +1475,16 @@
         <v>4</v>
       </c>
       <c r="J5" t="s">
+        <v>41</v>
+      </c>
+      <c r="K5" t="s">
         <v>42</v>
       </c>
-      <c r="K5" t="s">
+      <c r="L5" t="s">
         <v>43</v>
       </c>
-      <c r="L5" t="s">
-        <v>44</v>
-      </c>
       <c r="M5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="N5">
         <v>26</v>
@@ -1329,12 +1499,12 @@
         <v>28</v>
       </c>
       <c r="R5" t="s">
-        <v>150</v>
+        <v>126</v>
       </c>
     </row>
     <row r="6" spans="1:18">
       <c r="A6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B6" t="s">
         <v>20</v>
@@ -1361,22 +1531,22 @@
         <v>4</v>
       </c>
       <c r="J6" t="s">
+        <v>45</v>
+      </c>
+      <c r="K6" t="s">
         <v>46</v>
       </c>
-      <c r="K6" t="s">
+      <c r="L6" t="s">
         <v>47</v>
       </c>
-      <c r="L6" t="s">
+      <c r="M6" t="s">
         <v>48</v>
-      </c>
-      <c r="M6" t="s">
-        <v>49</v>
       </c>
       <c r="N6">
         <v>7</v>
       </c>
       <c r="O6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="Q6" t="s">
         <v>28</v>
@@ -1387,40 +1557,40 @@
         <v>18</v>
       </c>
       <c r="B7" t="s">
+        <v>51</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7" t="s">
+        <v>26</v>
+      </c>
+      <c r="H7" t="s">
+        <v>26</v>
+      </c>
+      <c r="I7" t="s">
+        <v>4</v>
+      </c>
+      <c r="J7" t="s">
         <v>52</v>
       </c>
-      <c r="C7">
-        <v>0</v>
-      </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
-      <c r="E7">
-        <v>0</v>
-      </c>
-      <c r="F7">
-        <v>0</v>
-      </c>
-      <c r="G7" t="s">
-        <v>26</v>
-      </c>
-      <c r="H7" t="s">
-        <v>26</v>
-      </c>
-      <c r="I7" t="s">
-        <v>4</v>
-      </c>
-      <c r="J7" t="s">
+      <c r="K7" t="s">
         <v>53</v>
       </c>
-      <c r="K7" t="s">
+      <c r="L7" t="s">
         <v>54</v>
       </c>
-      <c r="L7" t="s">
-        <v>55</v>
-      </c>
       <c r="M7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="N7">
         <v>26</v>
@@ -1435,7 +1605,7 @@
         <v>28</v>
       </c>
       <c r="R7" t="s">
-        <v>151</v>
+        <v>127</v>
       </c>
     </row>
     <row r="8" spans="1:18">
@@ -1455,7 +1625,7 @@
         <v>0</v>
       </c>
       <c r="F8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G8" t="s">
         <v>26</v>
@@ -1467,16 +1637,16 @@
         <v>4</v>
       </c>
       <c r="J8" t="s">
+        <v>55</v>
+      </c>
+      <c r="K8" t="s">
         <v>56</v>
       </c>
-      <c r="K8" t="s">
+      <c r="L8" t="s">
         <v>57</v>
       </c>
-      <c r="L8" t="s">
+      <c r="M8" t="s">
         <v>58</v>
-      </c>
-      <c r="M8" t="s">
-        <v>59</v>
       </c>
       <c r="N8">
         <v>26</v>
@@ -1508,7 +1678,7 @@
         <v>0</v>
       </c>
       <c r="F9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G9" t="s">
         <v>26</v>
@@ -1520,16 +1690,16 @@
         <v>4</v>
       </c>
       <c r="J9" t="s">
-        <v>152</v>
+        <v>128</v>
       </c>
       <c r="K9" t="s">
-        <v>153</v>
+        <v>129</v>
       </c>
       <c r="L9" t="s">
-        <v>154</v>
+        <v>130</v>
       </c>
       <c r="M9" t="s">
-        <v>155</v>
+        <v>131</v>
       </c>
       <c r="N9">
         <v>26</v>
@@ -1540,11 +1710,11 @@
       <c r="P9">
         <v>4238</v>
       </c>
-      <c r="Q9" t="s">
-        <v>156</v>
+      <c r="Q9" s="6" t="s">
+        <v>132</v>
       </c>
       <c r="R9" t="s">
-        <v>157</v>
+        <v>133</v>
       </c>
     </row>
     <row r="10" spans="1:18">
@@ -1567,25 +1737,25 @@
         <v>0</v>
       </c>
       <c r="G10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I10" t="s">
         <v>4</v>
       </c>
       <c r="J10" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="K10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="L10" t="s">
         <v>29</v>
       </c>
       <c r="M10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="N10">
         <v>26</v>
@@ -1611,7 +1781,7 @@
         <v>0</v>
       </c>
       <c r="E11" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F11">
         <v>0</v>
@@ -1626,16 +1796,16 @@
         <v>4</v>
       </c>
       <c r="J11" t="s">
+        <v>60</v>
+      </c>
+      <c r="K11" t="s">
+        <v>70</v>
+      </c>
+      <c r="L11" t="s">
         <v>61</v>
       </c>
-      <c r="K11" t="s">
-        <v>72</v>
-      </c>
-      <c r="L11" t="s">
+      <c r="M11" t="s">
         <v>62</v>
-      </c>
-      <c r="M11" t="s">
-        <v>63</v>
       </c>
       <c r="N11">
         <v>26</v>
@@ -1650,7 +1820,7 @@
         <v>28</v>
       </c>
       <c r="R11" t="s">
-        <v>158</v>
+        <v>134</v>
       </c>
     </row>
     <row r="12" spans="1:18">
@@ -1682,16 +1852,16 @@
         <v>4</v>
       </c>
       <c r="J12" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="K12" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="L12" t="s">
+        <v>75</v>
+      </c>
+      <c r="M12" t="s">
         <v>77</v>
-      </c>
-      <c r="M12" t="s">
-        <v>79</v>
       </c>
       <c r="N12">
         <v>26</v>
@@ -1706,7 +1876,7 @@
         <v>28</v>
       </c>
       <c r="R12" t="s">
-        <v>159</v>
+        <v>135</v>
       </c>
     </row>
     <row r="13" spans="1:18">
@@ -1738,16 +1908,16 @@
         <v>4</v>
       </c>
       <c r="J13" t="s">
-        <v>160</v>
+        <v>136</v>
       </c>
       <c r="K13" t="s">
-        <v>161</v>
+        <v>137</v>
       </c>
       <c r="L13" t="s">
-        <v>162</v>
+        <v>138</v>
       </c>
       <c r="M13" t="s">
-        <v>163</v>
+        <v>139</v>
       </c>
       <c r="N13">
         <v>26</v>
@@ -1759,7 +1929,7 @@
         <v>4546</v>
       </c>
       <c r="Q13" t="s">
-        <v>164</v>
+        <v>140</v>
       </c>
     </row>
     <row r="14" spans="1:18">
@@ -1791,16 +1961,16 @@
         <v>4</v>
       </c>
       <c r="J14" t="s">
-        <v>130</v>
+        <v>114</v>
       </c>
       <c r="K14" t="s">
-        <v>165</v>
+        <v>141</v>
       </c>
       <c r="L14" t="s">
-        <v>166</v>
+        <v>142</v>
       </c>
       <c r="M14" t="s">
-        <v>163</v>
+        <v>139</v>
       </c>
       <c r="N14">
         <v>26</v>
@@ -1812,18 +1982,18 @@
         <v>3944</v>
       </c>
       <c r="Q14" t="s">
-        <v>167</v>
+        <v>143</v>
       </c>
     </row>
     <row r="15" spans="1:18">
       <c r="A15" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B15">
         <v>0</v>
       </c>
       <c r="E15" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F15">
         <v>0</v>
@@ -1838,22 +2008,22 @@
         <v>4</v>
       </c>
       <c r="J15" t="s">
+        <v>71</v>
+      </c>
+      <c r="K15" t="s">
+        <v>72</v>
+      </c>
+      <c r="L15" t="s">
         <v>73</v>
       </c>
-      <c r="K15" t="s">
-        <v>74</v>
-      </c>
-      <c r="L15" t="s">
-        <v>75</v>
-      </c>
       <c r="M15" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="N15">
         <v>18</v>
       </c>
       <c r="O15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="Q15" t="s">
         <v>28</v>
@@ -1861,7 +2031,7 @@
     </row>
     <row r="16" spans="1:18">
       <c r="A16" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B16" t="s">
         <v>20</v>
@@ -1888,28 +2058,28 @@
         <v>4</v>
       </c>
       <c r="J16" t="s">
+        <v>78</v>
+      </c>
+      <c r="K16" t="s">
+        <v>79</v>
+      </c>
+      <c r="L16" t="s">
         <v>80</v>
       </c>
-      <c r="K16" t="s">
+      <c r="M16" t="s">
         <v>81</v>
-      </c>
-      <c r="L16" t="s">
-        <v>82</v>
-      </c>
-      <c r="M16" t="s">
-        <v>83</v>
       </c>
       <c r="N16">
         <v>18</v>
       </c>
       <c r="O16" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="Q16" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="17" spans="1:17">
+    <row r="17" spans="1:18">
       <c r="A17" t="s">
         <v>18</v>
       </c>
@@ -1935,16 +2105,16 @@
         <v>4</v>
       </c>
       <c r="J17" t="s">
+        <v>82</v>
+      </c>
+      <c r="K17" t="s">
+        <v>83</v>
+      </c>
+      <c r="L17" t="s">
         <v>84</v>
       </c>
-      <c r="K17" t="s">
+      <c r="M17" t="s">
         <v>85</v>
-      </c>
-      <c r="L17" t="s">
-        <v>86</v>
-      </c>
-      <c r="M17" t="s">
-        <v>87</v>
       </c>
       <c r="N17">
         <v>26</v>
@@ -1956,24 +2126,24 @@
         <v>28</v>
       </c>
     </row>
-    <row r="18" spans="1:17">
+    <row r="18" spans="1:18">
       <c r="A18" t="s">
         <v>18</v>
       </c>
       <c r="I18" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="J18">
         <v>1</v>
       </c>
       <c r="K18" t="s">
+        <v>93</v>
+      </c>
+      <c r="L18" t="s">
+        <v>94</v>
+      </c>
+      <c r="M18" t="s">
         <v>95</v>
-      </c>
-      <c r="L18" t="s">
-        <v>96</v>
-      </c>
-      <c r="M18" t="s">
-        <v>97</v>
       </c>
       <c r="N18">
         <v>26</v>
@@ -1985,24 +2155,24 @@
         <v>28</v>
       </c>
     </row>
-    <row r="19" spans="1:17">
+    <row r="19" spans="1:18">
       <c r="A19" t="s">
         <v>18</v>
       </c>
       <c r="I19" t="s">
+        <v>103</v>
+      </c>
+      <c r="J19" t="s">
+        <v>104</v>
+      </c>
+      <c r="K19" t="s">
         <v>105</v>
       </c>
-      <c r="J19" t="s">
+      <c r="L19" t="s">
         <v>106</v>
       </c>
-      <c r="K19" t="s">
+      <c r="M19" t="s">
         <v>107</v>
-      </c>
-      <c r="L19" t="s">
-        <v>108</v>
-      </c>
-      <c r="M19" t="s">
-        <v>109</v>
       </c>
       <c r="N19">
         <v>26</v>
@@ -2015,6 +2185,115 @@
       </c>
       <c r="Q19" t="s">
         <v>28</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18">
+      <c r="A20" t="s">
+        <v>18</v>
+      </c>
+      <c r="B20">
+        <v>0</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
+      </c>
+      <c r="F20" t="s">
+        <v>51</v>
+      </c>
+      <c r="G20" t="s">
+        <v>26</v>
+      </c>
+      <c r="H20" t="s">
+        <v>26</v>
+      </c>
+      <c r="I20" t="s">
+        <v>4</v>
+      </c>
+      <c r="J20" t="s">
+        <v>167</v>
+      </c>
+      <c r="K20" t="s">
+        <v>168</v>
+      </c>
+      <c r="L20" t="s">
+        <v>177</v>
+      </c>
+      <c r="M20" t="s">
+        <v>166</v>
+      </c>
+      <c r="N20">
+        <v>26</v>
+      </c>
+      <c r="O20" t="s">
+        <v>38</v>
+      </c>
+      <c r="P20">
+        <v>3644</v>
+      </c>
+      <c r="Q20" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="R20" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18">
+      <c r="B21">
+        <v>0</v>
+      </c>
+      <c r="C21">
+        <v>0</v>
+      </c>
+      <c r="D21">
+        <v>0</v>
+      </c>
+      <c r="E21">
+        <v>0</v>
+      </c>
+      <c r="F21" t="s">
+        <v>51</v>
+      </c>
+      <c r="G21" t="s">
+        <v>26</v>
+      </c>
+      <c r="H21" t="s">
+        <v>26</v>
+      </c>
+      <c r="I21" t="s">
+        <v>4</v>
+      </c>
+      <c r="J21" t="s">
+        <v>182</v>
+      </c>
+      <c r="K21" t="s">
+        <v>183</v>
+      </c>
+      <c r="L21" t="s">
+        <v>184</v>
+      </c>
+      <c r="M21" t="s">
+        <v>185</v>
+      </c>
+      <c r="N21">
+        <v>26</v>
+      </c>
+      <c r="O21" t="s">
+        <v>38</v>
+      </c>
+      <c r="P21">
+        <v>3390</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>23</v>
+      </c>
+      <c r="R21" t="s">
+        <v>186</v>
       </c>
     </row>
     <row r="38" spans="1:15">
@@ -2040,185 +2319,162 @@
         <v>0</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>124</v>
+        <v>17</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>40</v>
+        <v>1</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="I39" s="1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J39" s="1" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="K39" s="1" t="s">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="L39" s="1" t="s">
-        <v>6</v>
+        <v>36</v>
       </c>
       <c r="M39" s="1" t="s">
-        <v>25</v>
+        <v>86</v>
       </c>
       <c r="N39" s="1" t="s">
-        <v>36</v>
+        <v>96</v>
       </c>
       <c r="O39" s="1" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="40" spans="1:15" ht="16">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15">
       <c r="A40" t="s">
-        <v>18</v>
-      </c>
-      <c r="C40" t="s">
-        <v>52</v>
-      </c>
-      <c r="D40">
-        <v>0</v>
-      </c>
-      <c r="E40" t="s">
-        <v>19</v>
-      </c>
-      <c r="F40" t="s">
-        <v>20</v>
-      </c>
-      <c r="G40">
-        <v>0</v>
-      </c>
-      <c r="H40" t="s">
-        <v>4</v>
-      </c>
-      <c r="I40" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="J40" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="K40" s="3" t="s">
-        <v>136</v>
-      </c>
-      <c r="L40" t="s">
-        <v>137</v>
-      </c>
-      <c r="M40">
-        <v>26</v>
+        <v>66</v>
+      </c>
+      <c r="J40" t="s">
+        <v>63</v>
       </c>
       <c r="N40" t="s">
-        <v>38</v>
-      </c>
-      <c r="O40" s="3">
-        <v>72.700999999999993</v>
+        <v>148</v>
       </c>
     </row>
     <row r="41" spans="1:15" ht="16">
       <c r="A41" t="s">
-        <v>18</v>
+        <v>67</v>
+      </c>
+      <c r="B41" t="s">
+        <v>51</v>
+      </c>
+      <c r="C41">
+        <v>0</v>
       </c>
       <c r="D41" t="s">
-        <v>52</v>
+        <v>19</v>
       </c>
       <c r="E41" t="s">
         <v>20</v>
       </c>
-      <c r="G41" t="s">
-        <v>19</v>
-      </c>
-      <c r="H41" t="s">
-        <v>4</v>
+      <c r="F41" t="s">
+        <v>4</v>
+      </c>
+      <c r="G41" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="H41" s="3" t="s">
+        <v>115</v>
       </c>
       <c r="I41" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="J41" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="K41" s="3" t="s">
-        <v>140</v>
+        <v>116</v>
+      </c>
+      <c r="J41" t="s">
+        <v>117</v>
+      </c>
+      <c r="K41">
+        <v>20</v>
       </c>
       <c r="L41" t="s">
-        <v>141</v>
-      </c>
-      <c r="M41">
-        <v>26</v>
+        <v>38</v>
+      </c>
+      <c r="M41" s="3">
+        <v>262.065</v>
       </c>
       <c r="N41" t="s">
-        <v>38</v>
-      </c>
-      <c r="O41" s="3">
-        <v>5.0039999999999996</v>
+        <v>148</v>
       </c>
     </row>
     <row r="42" spans="1:15">
       <c r="A42" t="s">
         <v>67</v>
       </c>
+      <c r="C42" t="s">
+        <v>20</v>
+      </c>
+      <c r="D42" t="s">
+        <v>19</v>
+      </c>
+      <c r="E42" t="s">
+        <v>51</v>
+      </c>
+      <c r="F42" t="s">
+        <v>4</v>
+      </c>
+      <c r="G42" t="s">
+        <v>87</v>
+      </c>
+      <c r="H42" t="s">
+        <v>76</v>
+      </c>
+      <c r="I42" t="s">
+        <v>88</v>
+      </c>
+      <c r="J42" t="s">
+        <v>89</v>
+      </c>
+      <c r="K42">
+        <v>20</v>
+      </c>
       <c r="L42" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="43" spans="1:15" ht="16">
+        <v>90</v>
+      </c>
+      <c r="M42">
+        <v>1162680</v>
+      </c>
+      <c r="N42" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15">
       <c r="A43" t="s">
-        <v>68</v>
-      </c>
-      <c r="C43" t="s">
-        <v>52</v>
-      </c>
-      <c r="D43">
-        <v>0</v>
-      </c>
-      <c r="E43" t="s">
-        <v>19</v>
+        <v>92</v>
       </c>
       <c r="F43" t="s">
-        <v>20</v>
-      </c>
-      <c r="G43">
-        <v>0</v>
-      </c>
-      <c r="H43" t="s">
-        <v>4</v>
-      </c>
-      <c r="I43" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="J43" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="K43" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="L43" t="s">
-        <v>133</v>
-      </c>
-      <c r="M43">
-        <v>20</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="M43" s="4"/>
       <c r="N43" t="s">
-        <v>38</v>
-      </c>
-      <c r="O43" s="3">
-        <v>262.065</v>
+        <v>148</v>
       </c>
     </row>
     <row r="44" spans="1:15">
       <c r="A44" t="s">
-        <v>68</v>
+        <v>18</v>
+      </c>
+      <c r="B44" t="s">
+        <v>149</v>
       </c>
       <c r="D44" t="s">
         <v>20</v>
@@ -2227,416 +2483,681 @@
         <v>19</v>
       </c>
       <c r="F44" t="s">
-        <v>52</v>
+        <v>4</v>
+      </c>
+      <c r="G44" t="s">
+        <v>170</v>
       </c>
       <c r="H44" t="s">
-        <v>4</v>
+        <v>171</v>
       </c>
       <c r="I44" t="s">
-        <v>89</v>
+        <v>172</v>
       </c>
       <c r="J44" t="s">
-        <v>78</v>
-      </c>
-      <c r="K44" t="s">
-        <v>90</v>
+        <v>169</v>
+      </c>
+      <c r="K44">
+        <v>26</v>
       </c>
       <c r="L44" t="s">
-        <v>91</v>
+        <v>102</v>
       </c>
       <c r="M44">
-        <v>20</v>
+        <v>3234</v>
       </c>
       <c r="N44" t="s">
-        <v>92</v>
-      </c>
-      <c r="O44">
-        <v>1162680</v>
+        <v>23</v>
+      </c>
+      <c r="O44" t="s">
+        <v>187</v>
       </c>
     </row>
     <row r="45" spans="1:15">
       <c r="A45" t="s">
-        <v>94</v>
-      </c>
-      <c r="O45" s="4" t="s">
-        <v>123</v>
+        <v>18</v>
+      </c>
+      <c r="C45" t="s">
+        <v>149</v>
+      </c>
+      <c r="D45" t="s">
+        <v>20</v>
+      </c>
+      <c r="E45" t="s">
+        <v>20</v>
+      </c>
+      <c r="F45" t="s">
+        <v>4</v>
+      </c>
+      <c r="G45">
+        <v>1</v>
+      </c>
+      <c r="H45" t="s">
+        <v>178</v>
+      </c>
+      <c r="I45" t="s">
+        <v>179</v>
+      </c>
+      <c r="J45" t="s">
+        <v>180</v>
+      </c>
+      <c r="K45">
+        <v>26</v>
+      </c>
+      <c r="L45" t="s">
+        <v>102</v>
+      </c>
+      <c r="M45">
+        <v>2471</v>
+      </c>
+      <c r="N45" t="s">
+        <v>23</v>
+      </c>
+      <c r="O45" t="s">
+        <v>181</v>
       </c>
     </row>
     <row r="46" spans="1:15">
       <c r="A46" t="s">
         <v>18</v>
       </c>
+      <c r="F46" t="s">
+        <v>108</v>
+      </c>
+      <c r="G46">
+        <v>1</v>
+      </c>
       <c r="H46" t="s">
-        <v>110</v>
-      </c>
-      <c r="I46">
-        <v>1</v>
+        <v>147</v>
+      </c>
+      <c r="I46" t="s">
+        <v>109</v>
       </c>
       <c r="J46" t="s">
-        <v>111</v>
-      </c>
-      <c r="K46" t="s">
-        <v>112</v>
+        <v>173</v>
+      </c>
+      <c r="K46">
+        <v>26</v>
       </c>
       <c r="L46" t="s">
-        <v>113</v>
+        <v>102</v>
       </c>
       <c r="M46">
-        <v>26</v>
+        <v>13041</v>
       </c>
       <c r="N46" t="s">
-        <v>38</v>
-      </c>
-      <c r="O46">
-        <v>9931</v>
+        <v>23</v>
+      </c>
+      <c r="O46" t="s">
+        <v>175</v>
       </c>
     </row>
     <row r="47" spans="1:15">
       <c r="A47" t="s">
         <v>18</v>
       </c>
+      <c r="B47" t="s">
+        <v>188</v>
+      </c>
+      <c r="D47" t="s">
+        <v>20</v>
+      </c>
+      <c r="E47" t="s">
+        <v>26</v>
+      </c>
+      <c r="F47" t="s">
+        <v>4</v>
+      </c>
+      <c r="G47" t="s">
+        <v>170</v>
+      </c>
       <c r="H47" t="s">
-        <v>110</v>
-      </c>
-      <c r="I47">
-        <v>1</v>
+        <v>171</v>
+      </c>
+      <c r="I47" t="s">
+        <v>172</v>
       </c>
       <c r="J47" t="s">
-        <v>111</v>
-      </c>
-      <c r="K47" t="s">
-        <v>112</v>
+        <v>189</v>
+      </c>
+      <c r="K47">
+        <v>26</v>
       </c>
       <c r="L47" t="s">
-        <v>118</v>
+        <v>102</v>
       </c>
       <c r="M47">
-        <v>26</v>
+        <v>3335</v>
       </c>
       <c r="N47" t="s">
-        <v>38</v>
-      </c>
-      <c r="O47">
-        <v>9856</v>
-      </c>
-    </row>
-    <row r="48" spans="1:15" ht="16">
+        <v>23</v>
+      </c>
+      <c r="O47" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15">
       <c r="A48" t="s">
         <v>18</v>
       </c>
+      <c r="C48" t="s">
+        <v>149</v>
+      </c>
       <c r="D48" t="s">
-        <v>52</v>
+        <v>20</v>
       </c>
       <c r="E48" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F48" t="s">
+        <v>4</v>
+      </c>
+      <c r="G48" t="s">
+        <v>191</v>
+      </c>
+      <c r="H48" t="s">
+        <v>192</v>
+      </c>
+      <c r="I48" t="s">
+        <v>193</v>
+      </c>
+      <c r="J48" t="s">
+        <v>194</v>
+      </c>
+      <c r="K48">
+        <v>26</v>
+      </c>
+      <c r="L48" t="s">
+        <v>102</v>
+      </c>
+      <c r="M48">
+        <v>4726</v>
+      </c>
+      <c r="N48" t="s">
+        <v>143</v>
+      </c>
+      <c r="O48" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14">
+      <c r="G49" t="s">
+        <v>196</v>
+      </c>
+      <c r="H49" t="s">
+        <v>192</v>
+      </c>
+      <c r="I49" t="s">
+        <v>193</v>
+      </c>
+      <c r="K49">
+        <v>26</v>
+      </c>
+      <c r="L49" t="s">
+        <v>102</v>
+      </c>
+      <c r="M49">
+        <v>4718</v>
+      </c>
+      <c r="N49" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="60" spans="1:14">
+      <c r="A60" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E60" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F60" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G60" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H60" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I60" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J60" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="K60" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="L60" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="M60" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="61" spans="1:14">
+      <c r="A61" t="s">
+        <v>18</v>
+      </c>
+      <c r="B61" t="s">
+        <v>28</v>
+      </c>
+      <c r="C61">
+        <v>0</v>
+      </c>
+      <c r="D61" t="s">
         <v>20</v>
       </c>
-      <c r="H48" t="s">
-        <v>4</v>
-      </c>
-      <c r="I48" t="s">
+      <c r="E61" t="s">
+        <v>4</v>
+      </c>
+      <c r="F61" t="s">
+        <v>29</v>
+      </c>
+      <c r="G61" t="s">
+        <v>30</v>
+      </c>
+      <c r="H61" t="s">
+        <v>31</v>
+      </c>
+      <c r="I61" t="s">
+        <v>32</v>
+      </c>
+      <c r="J61">
+        <v>26</v>
+      </c>
+      <c r="K61" t="s">
+        <v>102</v>
+      </c>
+      <c r="L61">
+        <v>8841</v>
+      </c>
+      <c r="M61" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="62" spans="1:14">
+      <c r="A62" t="s">
+        <v>18</v>
+      </c>
+      <c r="B62" t="s">
+        <v>28</v>
+      </c>
+      <c r="C62" t="s">
+        <v>28</v>
+      </c>
+      <c r="D62" t="s">
+        <v>20</v>
+      </c>
+      <c r="E62" t="s">
+        <v>4</v>
+      </c>
+      <c r="F62" t="s">
+        <v>98</v>
+      </c>
+      <c r="G62" t="s">
+        <v>99</v>
+      </c>
+      <c r="H62" t="s">
+        <v>100</v>
+      </c>
+      <c r="I62" t="s">
+        <v>101</v>
+      </c>
+      <c r="J62">
+        <v>26</v>
+      </c>
+      <c r="K62" t="s">
+        <v>102</v>
+      </c>
+      <c r="L62" s="2">
+        <v>5590</v>
+      </c>
+      <c r="M62" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="63" spans="1:14">
+      <c r="A63" t="s">
+        <v>18</v>
+      </c>
+      <c r="B63" t="s">
+        <v>97</v>
+      </c>
+      <c r="C63">
+        <v>0</v>
+      </c>
+      <c r="D63" t="s">
+        <v>59</v>
+      </c>
+      <c r="E63" t="s">
+        <v>4</v>
+      </c>
+      <c r="F63" t="s">
+        <v>110</v>
+      </c>
+      <c r="G63" t="s">
+        <v>111</v>
+      </c>
+      <c r="H63" t="s">
+        <v>112</v>
+      </c>
+      <c r="I63" t="s">
+        <v>113</v>
+      </c>
+      <c r="J63">
+        <v>26</v>
+      </c>
+      <c r="K63" t="s">
+        <v>102</v>
+      </c>
+      <c r="L63" s="2">
+        <v>6912</v>
+      </c>
+      <c r="M63" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="64" spans="1:14">
+      <c r="A64" t="s">
+        <v>18</v>
+      </c>
+      <c r="B64" t="s">
+        <v>118</v>
+      </c>
+      <c r="C64" t="s">
         <v>119</v>
       </c>
-      <c r="J48" t="s">
+      <c r="D64" t="s">
         <v>120</v>
       </c>
-      <c r="K48" t="s">
+      <c r="E64" t="s">
+        <v>4</v>
+      </c>
+      <c r="F64" t="s">
+        <v>145</v>
+      </c>
+      <c r="G64" t="s">
+        <v>123</v>
+      </c>
+      <c r="H64" t="s">
+        <v>146</v>
+      </c>
+      <c r="I64" t="s">
         <v>121</v>
       </c>
-      <c r="L48" t="s">
+      <c r="J64">
+        <v>26</v>
+      </c>
+      <c r="K64" t="s">
+        <v>102</v>
+      </c>
+      <c r="L64" s="2">
+        <v>3026</v>
+      </c>
+      <c r="M64" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="65" spans="1:14">
+      <c r="A65" t="s">
+        <v>18</v>
+      </c>
+      <c r="B65" t="s">
+        <v>118</v>
+      </c>
+      <c r="C65" t="s">
+        <v>97</v>
+      </c>
+      <c r="D65" t="s">
+        <v>59</v>
+      </c>
+      <c r="E65" t="s">
+        <v>4</v>
+      </c>
+      <c r="F65" t="s">
         <v>122</v>
       </c>
-      <c r="M48">
-        <v>20</v>
-      </c>
-      <c r="N48" t="s">
-        <v>70</v>
-      </c>
-      <c r="O48" s="3">
-        <v>1.6639999999999999</v>
-      </c>
-    </row>
-    <row r="49" spans="1:15" ht="16">
-      <c r="A49" t="s">
+      <c r="G65" t="s">
+        <v>123</v>
+      </c>
+      <c r="H65" t="s">
+        <v>124</v>
+      </c>
+      <c r="I65" t="s">
+        <v>139</v>
+      </c>
+      <c r="J65">
+        <v>26</v>
+      </c>
+      <c r="K65" t="s">
+        <v>102</v>
+      </c>
+      <c r="L65" s="2">
+        <v>3070</v>
+      </c>
+      <c r="M65" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="66" spans="1:14">
+      <c r="A66" t="s">
         <v>18</v>
       </c>
-      <c r="B49" t="s">
-        <v>52</v>
-      </c>
-      <c r="E49" t="s">
-        <v>19</v>
-      </c>
-      <c r="F49" t="s">
-        <v>20</v>
-      </c>
-      <c r="H49" t="s">
-        <v>4</v>
-      </c>
-      <c r="I49" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="J49" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="K49" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="L49" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="N49" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="O49" s="3">
-        <v>37.241999999999997</v>
-      </c>
-    </row>
-    <row r="54" spans="1:15">
-      <c r="A54" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B54" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C54" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D54" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E54" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F54" s="1" t="s">
+      <c r="B66" t="s">
+        <v>151</v>
+      </c>
+      <c r="C66" t="s">
+        <v>97</v>
+      </c>
+      <c r="D66" t="s">
+        <v>59</v>
+      </c>
+      <c r="E66" t="s">
+        <v>4</v>
+      </c>
+      <c r="F66" t="s">
+        <v>145</v>
+      </c>
+      <c r="G66" t="s">
+        <v>123</v>
+      </c>
+      <c r="H66" t="s">
+        <v>146</v>
+      </c>
+      <c r="I66" t="s">
+        <v>152</v>
+      </c>
+      <c r="J66">
+        <v>26</v>
+      </c>
+      <c r="K66" t="s">
+        <v>102</v>
+      </c>
+      <c r="L66" s="2">
+        <v>2940</v>
+      </c>
+      <c r="M66" t="s">
+        <v>150</v>
+      </c>
+      <c r="N66" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="67" spans="1:14">
+      <c r="A67" t="s">
+        <v>18</v>
+      </c>
+      <c r="B67" t="s">
+        <v>151</v>
+      </c>
+      <c r="C67" t="s">
+        <v>97</v>
+      </c>
+      <c r="D67" t="s">
+        <v>59</v>
+      </c>
+      <c r="E67" t="s">
+        <v>4</v>
+      </c>
+      <c r="F67" t="s">
+        <v>145</v>
+      </c>
+      <c r="G67" t="s">
+        <v>123</v>
+      </c>
+      <c r="H67" t="s">
+        <v>146</v>
+      </c>
+      <c r="I67" t="s">
+        <v>113</v>
+      </c>
+      <c r="J67">
+        <v>26</v>
+      </c>
+      <c r="K67" t="s">
+        <v>102</v>
+      </c>
+      <c r="L67" s="2">
+        <v>2938</v>
+      </c>
+      <c r="M67" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="68" spans="1:14">
+      <c r="A68" t="s">
+        <v>18</v>
+      </c>
+      <c r="B68" t="s">
+        <v>156</v>
+      </c>
+      <c r="C68" t="s">
+        <v>97</v>
+      </c>
+      <c r="D68" t="s">
+        <v>59</v>
+      </c>
+      <c r="E68" t="s">
+        <v>4</v>
+      </c>
+      <c r="F68" t="s">
+        <v>145</v>
+      </c>
+      <c r="G68" t="s">
+        <v>123</v>
+      </c>
+      <c r="H68" t="s">
+        <v>146</v>
+      </c>
+      <c r="I68" t="s">
+        <v>157</v>
+      </c>
+      <c r="J68">
+        <v>26</v>
+      </c>
+      <c r="K68" t="s">
+        <v>102</v>
+      </c>
+      <c r="L68" s="2">
+        <v>2928</v>
+      </c>
+      <c r="M68" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="69" spans="1:14">
+      <c r="A69" t="s">
+        <v>18</v>
+      </c>
+      <c r="B69" t="s">
+        <v>159</v>
+      </c>
+      <c r="C69" t="s">
+        <v>97</v>
+      </c>
+      <c r="D69" t="s">
+        <v>59</v>
+      </c>
+      <c r="E69" t="s">
+        <v>4</v>
+      </c>
+      <c r="F69" t="s">
+        <v>145</v>
+      </c>
+      <c r="G69" t="s">
+        <v>123</v>
+      </c>
+      <c r="H69" t="s">
+        <v>146</v>
+      </c>
+      <c r="I69" t="s">
+        <v>161</v>
+      </c>
+      <c r="J69">
+        <v>26</v>
+      </c>
+      <c r="K69" t="s">
+        <v>102</v>
+      </c>
+      <c r="L69" s="2">
+        <v>2915</v>
+      </c>
+      <c r="M69" s="5" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="70" spans="1:14">
+      <c r="A70" t="s">
+        <v>18</v>
+      </c>
+      <c r="B70" t="s">
+        <v>160</v>
+      </c>
+      <c r="C70" t="s">
+        <v>97</v>
+      </c>
+      <c r="D70" t="s">
+        <v>59</v>
+      </c>
+      <c r="E70" t="s">
+        <v>4</v>
+      </c>
+      <c r="F70">
         <v>1</v>
       </c>
-      <c r="G54" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="H54" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="I54" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="J54" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="K54" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="L54" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="M54" s="1" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="55" spans="1:15">
-      <c r="A55" t="s">
-        <v>18</v>
-      </c>
-      <c r="B55" t="s">
-        <v>28</v>
-      </c>
-      <c r="C55">
-        <v>0</v>
-      </c>
-      <c r="D55" t="s">
-        <v>20</v>
-      </c>
-      <c r="E55" t="s">
-        <v>4</v>
-      </c>
-      <c r="F55" t="s">
-        <v>29</v>
-      </c>
-      <c r="G55" t="s">
-        <v>30</v>
-      </c>
-      <c r="H55" t="s">
-        <v>31</v>
-      </c>
-      <c r="I55" t="s">
-        <v>32</v>
-      </c>
-      <c r="J55">
-        <v>26</v>
-      </c>
-      <c r="K55" t="s">
-        <v>104</v>
-      </c>
-      <c r="L55">
-        <v>8841</v>
-      </c>
-      <c r="M55" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="56" spans="1:15">
-      <c r="A56" t="s">
-        <v>18</v>
-      </c>
-      <c r="B56" t="s">
-        <v>28</v>
-      </c>
-      <c r="C56" t="s">
-        <v>28</v>
-      </c>
-      <c r="D56" t="s">
-        <v>20</v>
-      </c>
-      <c r="E56" t="s">
-        <v>4</v>
-      </c>
-      <c r="F56" t="s">
-        <v>100</v>
-      </c>
-      <c r="G56" t="s">
-        <v>101</v>
-      </c>
-      <c r="H56" t="s">
+      <c r="G70" t="s">
+        <v>163</v>
+      </c>
+      <c r="H70" t="s">
+        <v>164</v>
+      </c>
+      <c r="I70" t="s">
+        <v>162</v>
+      </c>
+      <c r="J70">
+        <v>26</v>
+      </c>
+      <c r="K70" t="s">
         <v>102</v>
       </c>
-      <c r="I56" t="s">
-        <v>103</v>
-      </c>
-      <c r="J56">
-        <v>26</v>
-      </c>
-      <c r="K56" t="s">
-        <v>104</v>
-      </c>
-      <c r="L56" s="2">
-        <v>5590</v>
-      </c>
-      <c r="M56" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="57" spans="1:15">
-      <c r="A57" t="s">
-        <v>18</v>
-      </c>
-      <c r="B57" t="s">
-        <v>99</v>
-      </c>
-      <c r="C57">
-        <v>0</v>
-      </c>
-      <c r="D57" t="s">
-        <v>60</v>
-      </c>
-      <c r="E57" t="s">
-        <v>4</v>
-      </c>
-      <c r="F57" t="s">
-        <v>114</v>
-      </c>
-      <c r="G57" t="s">
-        <v>115</v>
-      </c>
-      <c r="H57" t="s">
-        <v>116</v>
-      </c>
-      <c r="I57" t="s">
-        <v>117</v>
-      </c>
-      <c r="J57">
-        <v>26</v>
-      </c>
-      <c r="K57" t="s">
-        <v>104</v>
-      </c>
-      <c r="L57" s="2">
-        <v>6912</v>
-      </c>
-      <c r="M57" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="58" spans="1:15">
-      <c r="A58" t="s">
-        <v>18</v>
-      </c>
-      <c r="B58" t="s">
-        <v>142</v>
-      </c>
-      <c r="C58" t="s">
-        <v>143</v>
-      </c>
-      <c r="D58" t="s">
-        <v>144</v>
-      </c>
-      <c r="E58" t="s">
-        <v>4</v>
-      </c>
-      <c r="F58" t="s">
-        <v>169</v>
-      </c>
-      <c r="G58" t="s">
-        <v>147</v>
-      </c>
-      <c r="H58" t="s">
-        <v>170</v>
-      </c>
-      <c r="I58" t="s">
-        <v>145</v>
-      </c>
-      <c r="J58">
-        <v>26</v>
-      </c>
-      <c r="K58" t="s">
-        <v>104</v>
-      </c>
-      <c r="L58" s="2">
-        <v>3026</v>
-      </c>
-      <c r="M58" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="59" spans="1:15">
-      <c r="A59" t="s">
-        <v>18</v>
-      </c>
-      <c r="B59" t="s">
-        <v>142</v>
-      </c>
-      <c r="C59" t="s">
-        <v>99</v>
-      </c>
-      <c r="D59" t="s">
-        <v>60</v>
-      </c>
-      <c r="E59" t="s">
-        <v>4</v>
-      </c>
-      <c r="F59" t="s">
-        <v>146</v>
-      </c>
-      <c r="G59" t="s">
-        <v>147</v>
-      </c>
-      <c r="H59" t="s">
-        <v>148</v>
-      </c>
-      <c r="I59" t="s">
-        <v>163</v>
-      </c>
-      <c r="J59">
-        <v>26</v>
-      </c>
-      <c r="K59" t="s">
-        <v>104</v>
-      </c>
-      <c r="L59" s="2">
-        <v>3070</v>
-      </c>
-      <c r="M59" t="s">
-        <v>168</v>
+      <c r="L70" s="2">
+        <v>2023</v>
+      </c>
+      <c r="M70" t="s">
+        <v>158</v>
+      </c>
+      <c r="N70" t="s">
+        <v>165</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
FIFA -API identity resolution improved
</commit_message>
<xml_diff>
--- a/IdentityResolutionExperimentation/identity_resolution_results.xlsx
+++ b/IdentityResolutionExperimentation/identity_resolution_results.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26621"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22130"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\linar\OneDrive\Документы\GitHub\WDI_2019\IdentityResolutionExperimentation\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8DAB121-1E7B-4857-BEE5-467F3656DEDE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blatt2" sheetId="2" r:id="rId1"/>
@@ -19,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="461" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1875" uniqueCount="213">
   <si>
     <t>Blocker</t>
   </si>
@@ -591,9 +597,6 @@
     <t>3 Minutes 7 Secondes</t>
   </si>
   <si>
-    <t>160 wronf</t>
-  </si>
-  <si>
     <t>0.9850</t>
   </si>
   <si>
@@ -610,13 +613,64 @@
   </si>
   <si>
     <t>0.985</t>
+  </si>
+  <si>
+    <t>115 wrong</t>
+  </si>
+  <si>
+    <t>0.9853</t>
+  </si>
+  <si>
+    <t>0.7053</t>
+  </si>
+  <si>
+    <t>0.8221</t>
+  </si>
+  <si>
+    <t>2 Minutes 25 Seconds</t>
+  </si>
+  <si>
+    <t>245 wrong</t>
+  </si>
+  <si>
+    <t>0.9789</t>
+  </si>
+  <si>
+    <t>0.7316</t>
+  </si>
+  <si>
+    <t>0.8373</t>
+  </si>
+  <si>
+    <t>2 Minutes 23 Seconds</t>
+  </si>
+  <si>
+    <t>322 wrong</t>
+  </si>
+  <si>
+    <t>160 wrong</t>
+  </si>
+  <si>
+    <t>2 Minutes 21 Seconds</t>
+  </si>
+  <si>
+    <t>0.7873</t>
+  </si>
+  <si>
+    <t>0.6526</t>
+  </si>
+  <si>
+    <t>0.9920</t>
+  </si>
+  <si>
+    <t>50 wrong</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="6">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -661,7 +715,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -671,6 +725,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -797,7 +857,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -807,119 +867,120 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="111">
-    <cellStyle name="Besuchter Link" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="16" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="18" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="20" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="22" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="24" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="26" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="28" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="30" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="32" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="34" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="36" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="38" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="40" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="42" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="44" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="46" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="48" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="50" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="52" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="54" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="56" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="58" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="60" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="62" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="64" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="66" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="68" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="70" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="72" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="74" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="76" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="78" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="80" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="82" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="84" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="86" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="88" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="90" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="92" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="94" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="96" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="98" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="100" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="102" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="104" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="106" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="108" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="110" builtinId="9" hidden="1"/>
-    <cellStyle name="Link" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="7" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="9" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="11" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="13" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="15" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="17" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="19" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="21" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="23" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="25" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="27" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="29" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="31" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="33" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="35" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="37" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="39" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="41" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="43" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="45" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="47" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="49" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="51" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="53" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="55" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="57" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="59" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="61" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="63" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="65" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="67" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="69" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="71" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="73" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="75" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="77" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="79" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="81" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="83" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="85" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="87" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="89" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="91" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="93" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="95" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="97" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="99" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="101" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="103" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="105" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="107" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="109" builtinId="8" hidden="1"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Гиперссылка" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="93" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="95" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="97" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="99" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="101" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="103" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="105" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="107" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="109" builtinId="8" hidden="1"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="98" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="100" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="104" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="106" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="108" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="110" builtinId="9" hidden="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -1255,14 +1316,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E27" zoomScale="75" workbookViewId="0">
-      <selection activeCell="O61" sqref="O61"/>
+    <sheetView tabSelected="1" topLeftCell="J39" zoomScale="75" workbookViewId="0">
+      <selection activeCell="O52" sqref="A52:O52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
   <cols>
     <col min="1" max="1" width="44.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="44.33203125" customWidth="1"/>
@@ -2372,7 +2433,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="41" spans="1:15" ht="16">
+    <row r="41" spans="1:15">
       <c r="A41" t="s">
         <v>67</v>
       </c>
@@ -2514,46 +2575,47 @@
       </c>
     </row>
     <row r="45" spans="1:15">
-      <c r="A45" t="s">
+      <c r="A45" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C45" t="s">
+      <c r="B45" s="7"/>
+      <c r="C45" s="7" t="s">
         <v>149</v>
       </c>
-      <c r="D45" t="s">
+      <c r="D45" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="E45" t="s">
+      <c r="E45" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="F45" t="s">
-        <v>4</v>
-      </c>
-      <c r="G45">
+      <c r="F45" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="G45" s="7">
         <v>1</v>
       </c>
-      <c r="H45" t="s">
+      <c r="H45" s="7" t="s">
         <v>178</v>
       </c>
-      <c r="I45" t="s">
+      <c r="I45" s="7" t="s">
         <v>179</v>
       </c>
-      <c r="J45" t="s">
+      <c r="J45" s="7" t="s">
         <v>180</v>
       </c>
-      <c r="K45">
-        <v>26</v>
-      </c>
-      <c r="L45" t="s">
+      <c r="K45" s="7">
+        <v>26</v>
+      </c>
+      <c r="L45" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="M45">
+      <c r="M45" s="7">
         <v>2471</v>
       </c>
-      <c r="N45" t="s">
+      <c r="N45" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="O45" t="s">
+      <c r="O45" s="7" t="s">
         <v>181</v>
       </c>
     </row>
@@ -2633,7 +2695,7 @@
         <v>23</v>
       </c>
       <c r="O47" t="s">
-        <v>190</v>
+        <v>207</v>
       </c>
     </row>
     <row r="48" spans="1:15">
@@ -2653,16 +2715,16 @@
         <v>4</v>
       </c>
       <c r="G48" t="s">
+        <v>190</v>
+      </c>
+      <c r="H48" t="s">
         <v>191</v>
       </c>
-      <c r="H48" t="s">
+      <c r="I48" t="s">
         <v>192</v>
       </c>
-      <c r="I48" t="s">
+      <c r="J48" t="s">
         <v>193</v>
-      </c>
-      <c r="J48" t="s">
-        <v>194</v>
       </c>
       <c r="K48">
         <v>26</v>
@@ -2677,18 +2739,36 @@
         <v>143</v>
       </c>
       <c r="O48" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="49" spans="1:15">
+      <c r="A49" t="s">
+        <v>18</v>
+      </c>
+      <c r="C49" t="s">
+        <v>149</v>
+      </c>
+      <c r="D49" t="s">
+        <v>20</v>
+      </c>
+      <c r="E49" t="s">
+        <v>20</v>
+      </c>
+      <c r="F49" t="s">
+        <v>4</v>
+      </c>
+      <c r="G49" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="49" spans="1:14">
-      <c r="G49" t="s">
-        <v>196</v>
-      </c>
       <c r="H49" t="s">
+        <v>191</v>
+      </c>
+      <c r="I49" t="s">
         <v>192</v>
       </c>
-      <c r="I49" t="s">
-        <v>193</v>
+      <c r="J49" t="s">
+        <v>180</v>
       </c>
       <c r="K49">
         <v>26</v>
@@ -2702,8 +2782,188 @@
       <c r="N49" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="60" spans="1:14">
+      <c r="O49" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="50" spans="1:15">
+      <c r="A50" t="s">
+        <v>18</v>
+      </c>
+      <c r="C50" t="s">
+        <v>51</v>
+      </c>
+      <c r="D50" t="s">
+        <v>20</v>
+      </c>
+      <c r="E50" t="s">
+        <v>26</v>
+      </c>
+      <c r="F50" t="s">
+        <v>4</v>
+      </c>
+      <c r="G50" t="s">
+        <v>197</v>
+      </c>
+      <c r="H50" t="s">
+        <v>198</v>
+      </c>
+      <c r="I50" t="s">
+        <v>199</v>
+      </c>
+      <c r="J50" t="s">
+        <v>200</v>
+      </c>
+      <c r="K50">
+        <v>26</v>
+      </c>
+      <c r="L50" t="s">
+        <v>102</v>
+      </c>
+      <c r="M50">
+        <v>5108</v>
+      </c>
+      <c r="N50" t="s">
+        <v>144</v>
+      </c>
+      <c r="O50" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="51" spans="1:15">
+      <c r="A51" t="s">
+        <v>18</v>
+      </c>
+      <c r="C51" t="s">
+        <v>51</v>
+      </c>
+      <c r="D51" t="s">
+        <v>20</v>
+      </c>
+      <c r="E51" t="s">
+        <v>26</v>
+      </c>
+      <c r="F51" t="s">
+        <v>4</v>
+      </c>
+      <c r="G51" t="s">
+        <v>202</v>
+      </c>
+      <c r="H51" t="s">
+        <v>203</v>
+      </c>
+      <c r="I51" t="s">
+        <v>204</v>
+      </c>
+      <c r="J51" t="s">
+        <v>205</v>
+      </c>
+      <c r="K51">
+        <v>26</v>
+      </c>
+      <c r="L51" t="s">
+        <v>102</v>
+      </c>
+      <c r="M51">
+        <v>5359</v>
+      </c>
+      <c r="N51" t="s">
+        <v>143</v>
+      </c>
+      <c r="O51" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="52" spans="1:15">
+      <c r="A52" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B52" s="5"/>
+      <c r="C52" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="D52" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E52" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F52" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G52" s="5" t="s">
+        <v>211</v>
+      </c>
+      <c r="H52" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="I52" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="J52" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="K52" s="5">
+        <v>26</v>
+      </c>
+      <c r="L52" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="M52" s="5">
+        <v>4371</v>
+      </c>
+      <c r="N52" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="O52" s="5" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="53" spans="1:15">
+      <c r="A53" t="s">
+        <v>18</v>
+      </c>
+      <c r="C53" t="s">
+        <v>149</v>
+      </c>
+      <c r="D53" t="s">
+        <v>20</v>
+      </c>
+      <c r="E53" t="s">
+        <v>20</v>
+      </c>
+      <c r="F53" t="s">
+        <v>4</v>
+      </c>
+      <c r="G53" t="s">
+        <v>211</v>
+      </c>
+      <c r="H53" t="s">
+        <v>210</v>
+      </c>
+      <c r="I53" t="s">
+        <v>209</v>
+      </c>
+      <c r="J53" t="s">
+        <v>208</v>
+      </c>
+      <c r="K53">
+        <v>26</v>
+      </c>
+      <c r="L53" t="s">
+        <v>102</v>
+      </c>
+      <c r="M53">
+        <v>4370</v>
+      </c>
+      <c r="N53" t="s">
+        <v>125</v>
+      </c>
+      <c r="O53" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="60" spans="1:15">
       <c r="A60" s="1" t="s">
         <v>0</v>
       </c>
@@ -2744,7 +3004,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="61" spans="1:14">
+    <row r="61" spans="1:15">
       <c r="A61" t="s">
         <v>18</v>
       </c>
@@ -2785,7 +3045,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="62" spans="1:14">
+    <row r="62" spans="1:15">
       <c r="A62" t="s">
         <v>18</v>
       </c>
@@ -2826,7 +3086,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="63" spans="1:14">
+    <row r="63" spans="1:15">
       <c r="A63" t="s">
         <v>18</v>
       </c>
@@ -2867,7 +3127,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="64" spans="1:14">
+    <row r="64" spans="1:15">
       <c r="A64" t="s">
         <v>18</v>
       </c>

</xml_diff>